<commit_message>
made some signal adjusts and started control
</commit_message>
<xml_diff>
--- a/SingleCycleProcessor_ControlSignals.xlsx
+++ b/SingleCycleProcessor_ControlSignals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="84">
   <si>
     <t xml:space="preserve">Instruction</t>
   </si>
@@ -270,6 +270,9 @@
     <t xml:space="preserve">"000100"</t>
   </si>
   <si>
+    <t xml:space="preserve">“-”</t>
+  </si>
+  <si>
     <t xml:space="preserve">01[]</t>
   </si>
   <si>
@@ -280,6 +283,9 @@
   </si>
   <si>
     <t xml:space="preserve">j</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"–-"</t>
   </si>
   <si>
     <t xml:space="preserve">jal</t>
@@ -295,7 +301,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -317,6 +323,15 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -375,7 +390,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -394,6 +409,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -423,12 +442,12 @@
   </sheetPr>
   <dimension ref="A1:AMJ35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O12" activeCellId="0" sqref="O12"/>
+      <selection pane="bottomRight" activeCell="F39" activeCellId="0" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -440,7 +459,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="12.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.88"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="1" width="10.8"/>
   </cols>
@@ -526,6 +545,7 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
+      <c r="E3" s="5"/>
       <c r="J3" s="1" t="s">
         <v>18</v>
       </c>
@@ -2751,7 +2771,7 @@
       <c r="D8" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="E8" s="6"/>
       <c r="F8" s="1" t="n">
         <v>0</v>
       </c>
@@ -2890,7 +2910,7 @@
       <c r="D11" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E11" s="6"/>
       <c r="F11" s="1" t="n">
         <v>0</v>
       </c>
@@ -2935,7 +2955,7 @@
       <c r="D12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E12" s="5"/>
+      <c r="E12" s="6"/>
       <c r="F12" s="1" t="n">
         <v>0</v>
       </c>
@@ -2980,7 +3000,7 @@
       <c r="D13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E13" s="5"/>
+      <c r="E13" s="6"/>
       <c r="F13" s="1" t="n">
         <v>0</v>
       </c>
@@ -3156,7 +3176,7 @@
       <c r="K18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L18" s="5" t="n">
+      <c r="L18" s="6" t="n">
         <v>11</v>
       </c>
       <c r="M18" s="1" t="n">
@@ -3206,7 +3226,7 @@
       <c r="K19" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L19" s="5" t="n">
+      <c r="L19" s="6" t="n">
         <v>11</v>
       </c>
       <c r="M19" s="1" t="n">
@@ -3253,7 +3273,7 @@
       <c r="K20" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L20" s="5" t="n">
+      <c r="L20" s="6" t="n">
         <v>11</v>
       </c>
       <c r="M20" s="1" t="n">
@@ -3279,7 +3299,7 @@
       <c r="D21" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E21" s="5"/>
+      <c r="E21" s="6"/>
       <c r="F21" s="1" t="n">
         <v>0</v>
       </c>
@@ -3298,7 +3318,7 @@
       <c r="K21" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L21" s="5" t="n">
+      <c r="L21" s="6" t="n">
         <v>11</v>
       </c>
       <c r="M21" s="1" t="n">
@@ -3377,8 +3397,8 @@
       <c r="F23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G23" s="1" t="n">
-        <v>1</v>
+      <c r="G23" s="7" t="n">
+        <v>0</v>
       </c>
       <c r="H23" s="1" t="n">
         <v>1</v>
@@ -3418,7 +3438,7 @@
       <c r="D24" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E24" s="5"/>
+      <c r="E24" s="6"/>
       <c r="F24" s="1" t="n">
         <v>0</v>
       </c>
@@ -3437,7 +3457,7 @@
       <c r="K24" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L24" s="5" t="n">
+      <c r="L24" s="6" t="n">
         <v>11</v>
       </c>
       <c r="M24" s="1" t="n">
@@ -3484,7 +3504,7 @@
       <c r="K25" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L25" s="5" t="n">
+      <c r="L25" s="6" t="n">
         <v>11</v>
       </c>
       <c r="M25" s="1" t="n">
@@ -3531,7 +3551,7 @@
       <c r="K26" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L26" s="5" t="n">
+      <c r="L26" s="6" t="n">
         <v>11</v>
       </c>
       <c r="M26" s="1" t="n">
@@ -3543,9 +3563,6 @@
       <c r="O26" s="1" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
@@ -3562,8 +3579,8 @@
       <c r="C29" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="1" t="n">
-        <v>0</v>
+      <c r="D29" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>47</v>
@@ -3587,7 +3604,7 @@
         <v>1</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M29" s="1" t="n">
         <v>0</v>
@@ -3601,16 +3618,16 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="1" t="n">
-        <v>0</v>
+      <c r="D30" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>47</v>
@@ -3634,7 +3651,7 @@
         <v>1</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M30" s="1" t="n">
         <v>0</v>
@@ -3653,7 +3670,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>42</v>
@@ -3661,10 +3678,10 @@
       <c r="C33" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E33" s="5"/>
+      <c r="D33" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E33" s="6"/>
       <c r="F33" s="1" t="n">
         <v>0</v>
       </c>
@@ -3683,7 +3700,9 @@
       <c r="K33" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L33" s="5"/>
+      <c r="L33" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="M33" s="1" t="n">
         <v>1</v>
       </c>
@@ -3696,7 +3715,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>44</v>
@@ -3704,10 +3723,10 @@
       <c r="C34" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D34" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E34" s="5"/>
+      <c r="D34" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E34" s="6"/>
       <c r="F34" s="1" t="n">
         <v>0</v>
       </c>
@@ -3726,7 +3745,9 @@
       <c r="K34" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L34" s="5"/>
+      <c r="L34" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="M34" s="1" t="n">
         <v>0</v>
       </c>
@@ -3739,7 +3760,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>20</v>
@@ -3747,10 +3768,10 @@
       <c r="C35" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E35" s="5"/>
+      <c r="D35" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E35" s="6"/>
       <c r="F35" s="1" t="n">
         <v>0</v>
       </c>
@@ -3763,7 +3784,7 @@
       <c r="I35" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="J35" s="5" t="n">
+      <c r="J35" s="6" t="n">
         <v>1</v>
       </c>
       <c r="K35" s="1" t="n">

</xml_diff>

<commit_message>
the grind has begun
</commit_message>
<xml_diff>
--- a/SingleCycleProcessor_ControlSignals.xlsx
+++ b/SingleCycleProcessor_ControlSignals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="86">
   <si>
     <t xml:space="preserve">Instruction</t>
   </si>
@@ -292,6 +292,12 @@
   </si>
   <si>
     <t xml:space="preserve">jr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Halt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“010100”</t>
   </si>
 </sst>
 </file>
@@ -390,7 +396,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -419,10 +425,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,14 +442,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ35"/>
+  <dimension ref="A1:AMJ37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F39" activeCellId="0" sqref="F39"/>
+      <selection pane="bottomRight" activeCell="E40" activeCellId="0" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3397,7 +3399,7 @@
       <c r="F23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G23" s="7" t="n">
+      <c r="G23" s="1" t="n">
         <v>0</v>
       </c>
       <c r="H23" s="1" t="n">
@@ -3801,6 +3803,17 @@
       </c>
       <c r="O35" s="1" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"fixed concating and filled in some gaps"
</commit_message>
<xml_diff>
--- a/SingleCycleProcessor_ControlSignals.xlsx
+++ b/SingleCycleProcessor_ControlSignals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="90">
   <si>
     <t xml:space="preserve">Instruction</t>
   </si>
@@ -207,6 +207,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">11 [i-instr]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Note: other signals you may have must be correctly assigned for the add; if you redefined these signals, you probably will need to change the sample values</t>
   </si>
   <si>
@@ -294,10 +297,19 @@
     <t xml:space="preserve">jr</t>
   </si>
   <si>
+    <t xml:space="preserve">Indicates to the sim that the intended program exe is done</t>
+  </si>
+  <si>
     <t xml:space="preserve">Halt</t>
   </si>
   <si>
     <t xml:space="preserve">“010100”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“----”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“–”</t>
   </si>
 </sst>
 </file>
@@ -396,7 +408,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -425,6 +437,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,14 +458,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ37"/>
+  <dimension ref="A1:AMJ38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E40" activeCellId="0" sqref="E40"/>
+      <selection pane="bottomRight" activeCell="T32" activeCellId="0" sqref="T32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3178,8 +3194,8 @@
       <c r="K18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L18" s="6" t="n">
-        <v>11</v>
+      <c r="L18" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="M18" s="1" t="n">
         <v>0</v>
@@ -3191,15 +3207,15 @@
         <v>0</v>
       </c>
       <c r="P18" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>53</v>
@@ -3228,8 +3244,8 @@
       <c r="K19" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L19" s="6" t="n">
-        <v>11</v>
+      <c r="L19" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="M19" s="1" t="n">
         <v>0</v>
@@ -3243,10 +3259,10 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>53</v>
@@ -3275,8 +3291,8 @@
       <c r="K20" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L20" s="6" t="n">
-        <v>11</v>
+      <c r="L20" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="M20" s="1" t="n">
         <v>0</v>
@@ -3290,10 +3306,10 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>53</v>
@@ -3320,8 +3336,8 @@
       <c r="K21" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L21" s="6" t="n">
-        <v>11</v>
+      <c r="L21" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="M21" s="1" t="n">
         <v>0</v>
@@ -3335,7 +3351,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>49</v>
@@ -3347,7 +3363,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F22" s="1" t="n">
         <v>1</v>
@@ -3368,7 +3384,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="M22" s="1" t="n">
         <v>0</v>
@@ -3382,10 +3398,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>53</v>
@@ -3394,7 +3410,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F23" s="1" t="n">
         <v>0</v>
@@ -3415,7 +3431,7 @@
         <v>0</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="M23" s="1" t="n">
         <v>0</v>
@@ -3429,13 +3445,13 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>1</v>
@@ -3459,8 +3475,8 @@
       <c r="K24" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L24" s="6" t="n">
-        <v>11</v>
+      <c r="L24" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="M24" s="1" t="n">
         <v>0</v>
@@ -3474,10 +3490,10 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>53</v>
@@ -3506,8 +3522,8 @@
       <c r="K25" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L25" s="6" t="n">
-        <v>11</v>
+      <c r="L25" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="M25" s="1" t="n">
         <v>0</v>
@@ -3521,10 +3537,10 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>53</v>
@@ -3553,8 +3569,8 @@
       <c r="K26" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L26" s="6" t="n">
-        <v>11</v>
+      <c r="L26" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="M26" s="1" t="n">
         <v>0</v>
@@ -3573,16 +3589,16 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>47</v>
@@ -3606,7 +3622,7 @@
         <v>1</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M29" s="1" t="n">
         <v>0</v>
@@ -3620,16 +3636,16 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>47</v>
@@ -3653,7 +3669,7 @@
         <v>1</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M30" s="1" t="n">
         <v>0</v>
@@ -3672,7 +3688,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>42</v>
@@ -3681,7 +3697,7 @@
         <v>53</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="1" t="n">
@@ -3703,7 +3719,7 @@
         <v>0</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M33" s="1" t="n">
         <v>1</v>
@@ -3717,7 +3733,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>44</v>
@@ -3726,7 +3742,7 @@
         <v>53</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="1" t="n">
@@ -3748,7 +3764,7 @@
         <v>0</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M34" s="1" t="n">
         <v>0</v>
@@ -3762,7 +3778,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>20</v>
@@ -3771,7 +3787,7 @@
         <v>52</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="1" t="n">
@@ -3805,23 +3821,73 @@
         <v>0</v>
       </c>
     </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="6"/>
+      <c r="J36" s="6"/>
+    </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B37" s="1" t="s">
+      <c r="A37" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>53</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:U1"/>
+    <mergeCell ref="A37:E37"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
worked on ALUOp signals and added halt instr
</commit_message>
<xml_diff>
--- a/SingleCycleProcessor_ControlSignals.xlsx
+++ b/SingleCycleProcessor_ControlSignals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="100">
   <si>
     <t xml:space="preserve">Instruction</t>
   </si>
@@ -70,12 +70,18 @@
     <t xml:space="preserve">Link</t>
   </si>
   <si>
+    <t xml:space="preserve">Halt</t>
+  </si>
+  <si>
     <t xml:space="preserve">Note: these are example control signals from the text and your skeleton code; you will need to add more control signals; you may rename any control signals, except those given in the skeleton code.</t>
   </si>
   <si>
     <t xml:space="preserve">R-type</t>
   </si>
   <si>
+    <t xml:space="preserve">Output depends on ALU implementation</t>
+  </si>
+  <si>
     <t xml:space="preserve">(0=rt, 1=rd)</t>
   </si>
   <si>
@@ -91,7 +97,7 @@
     <t xml:space="preserve">0010 [A + B]</t>
   </si>
   <si>
-    <t xml:space="preserve">10 [R-instr]</t>
+    <t xml:space="preserve">0001 [add]</t>
   </si>
   <si>
     <t xml:space="preserve">add</t>
@@ -109,12 +115,18 @@
     <t xml:space="preserve">0000 []</t>
   </si>
   <si>
+    <t xml:space="preserve">0010 [and]</t>
+  </si>
+  <si>
     <t xml:space="preserve">nor</t>
   </si>
   <si>
     <t xml:space="preserve">"100111"</t>
   </si>
   <si>
+    <t xml:space="preserve">0011 [nor]</t>
+  </si>
+  <si>
     <t xml:space="preserve">xor</t>
   </si>
   <si>
@@ -124,6 +136,9 @@
     <t xml:space="preserve">“100110”</t>
   </si>
   <si>
+    <t xml:space="preserve">0100 [xor]</t>
+  </si>
+  <si>
     <t xml:space="preserve">or</t>
   </si>
   <si>
@@ -133,6 +148,9 @@
     <t xml:space="preserve">0001 []</t>
   </si>
   <si>
+    <t xml:space="preserve">0101 [or]</t>
+  </si>
+  <si>
     <t xml:space="preserve">slt</t>
   </si>
   <si>
@@ -142,21 +160,33 @@
     <t xml:space="preserve">0111 []</t>
   </si>
   <si>
+    <t xml:space="preserve">0110 [slt]</t>
+  </si>
+  <si>
     <t xml:space="preserve">sll</t>
   </si>
   <si>
+    <t xml:space="preserve">0111 [sll]</t>
+  </si>
+  <si>
     <t xml:space="preserve">srl</t>
   </si>
   <si>
     <t xml:space="preserve">"000010"</t>
   </si>
   <si>
+    <t xml:space="preserve">1000 [srl]</t>
+  </si>
+  <si>
     <t xml:space="preserve">sra</t>
   </si>
   <si>
     <t xml:space="preserve">"000011"</t>
   </si>
   <si>
+    <t xml:space="preserve">1001 [sra]</t>
+  </si>
+  <si>
     <t xml:space="preserve">sub</t>
   </si>
   <si>
@@ -164,6 +194,9 @@
   </si>
   <si>
     <t xml:space="preserve">0110 []</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1010 [sub]</t>
   </si>
   <si>
     <t xml:space="preserve">subu</t>
@@ -207,9 +240,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">11 [i-instr]</t>
-  </si>
-  <si>
     <t xml:space="preserve">Note: other signals you may have must be correctly assigned for the add; if you redefined these signals, you probably will need to change the sample values</t>
   </si>
   <si>
@@ -231,13 +261,16 @@
     <t xml:space="preserve">"001111"</t>
   </si>
   <si>
+    <t xml:space="preserve">1101 [lui]</t>
+  </si>
+  <si>
     <t xml:space="preserve">lw</t>
   </si>
   <si>
     <t xml:space="preserve">0010 []</t>
   </si>
   <si>
-    <t xml:space="preserve">00[]</t>
+    <t xml:space="preserve">0000 [LS]</t>
   </si>
   <si>
     <t xml:space="preserve">sw</t>
@@ -276,7 +309,7 @@
     <t xml:space="preserve">“-”</t>
   </si>
   <si>
-    <t xml:space="preserve">01[]</t>
+    <t xml:space="preserve">1011 [beq]</t>
   </si>
   <si>
     <t xml:space="preserve">bne</t>
@@ -285,10 +318,13 @@
     <t xml:space="preserve">"000101"</t>
   </si>
   <si>
+    <t xml:space="preserve">1100 [bne]</t>
+  </si>
+  <si>
     <t xml:space="preserve">j</t>
   </si>
   <si>
-    <t xml:space="preserve">"–-"</t>
+    <t xml:space="preserve">1110 [Jumps]</t>
   </si>
   <si>
     <t xml:space="preserve">jal</t>
@@ -300,16 +336,10 @@
     <t xml:space="preserve">Indicates to the sim that the intended program exe is done</t>
   </si>
   <si>
-    <t xml:space="preserve">Halt</t>
-  </si>
-  <si>
     <t xml:space="preserve">“010100”</t>
   </si>
   <si>
-    <t xml:space="preserve">“----”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“–”</t>
+    <t xml:space="preserve">1111 [halt]??</t>
   </si>
 </sst>
 </file>
@@ -319,7 +349,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -341,15 +371,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -408,7 +429,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -433,8 +454,20 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -458,14 +491,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ38"/>
+  <dimension ref="A1:AMJ44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="T32" activeCellId="0" sqref="T32"/>
+      <selection pane="bottomRight" activeCell="K11" activeCellId="0" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -479,7 +512,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="12.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.88"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="1" width="10.8"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="17.22"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="13" style="1" width="10.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -512,6 +547,7 @@
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
       <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
@@ -553,19 +589,24 @@
       <c r="O2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="E3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="J3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="M3" s="1" t="n">
         <v>0</v>
@@ -576,23 +617,26 @@
       <c r="O3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P3" s="4"/>
+      <c r="P3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>22</v>
+      <c r="E4" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>0</v>
@@ -612,8 +656,8 @@
       <c r="K4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>23</v>
+      <c r="L4" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="M4" s="1" t="n">
         <v>0</v>
@@ -624,7 +668,9 @@
       <c r="O4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="T4" s="0"/>
+      <c r="P4" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="U4" s="0"/>
       <c r="V4" s="0"/>
       <c r="W4" s="0"/>
@@ -1632,41 +1678,41 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="F5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="M5" s="1" t="n">
         <v>0</v>
       </c>
@@ -1676,7 +1722,9 @@
       <c r="O5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="T5" s="0"/>
+      <c r="P5" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="U5" s="0"/>
       <c r="V5" s="0"/>
       <c r="W5" s="0"/>
@@ -2684,19 +2732,19 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>28</v>
+      <c r="E6" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>0</v>
@@ -2716,8 +2764,8 @@
       <c r="K6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>23</v>
+      <c r="L6" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="M6" s="1" t="n">
         <v>0</v>
@@ -2726,23 +2774,26 @@
         <v>0</v>
       </c>
       <c r="O6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="6" t="n">
         <v>1100</v>
       </c>
       <c r="F7" s="1" t="n">
@@ -2763,8 +2814,8 @@
       <c r="K7" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>23</v>
+      <c r="L7" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="M7" s="1" t="n">
         <v>0</v>
@@ -2773,18 +2824,21 @@
         <v>0</v>
       </c>
       <c r="O7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>0</v>
@@ -2808,8 +2862,8 @@
       <c r="K8" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>23</v>
+      <c r="L8" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="M8" s="1" t="n">
         <v>0</v>
@@ -2818,24 +2872,27 @@
         <v>0</v>
       </c>
       <c r="O8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>36</v>
+      <c r="E9" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>0</v>
@@ -2855,8 +2912,8 @@
       <c r="K9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>23</v>
+      <c r="L9" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="M9" s="1" t="n">
         <v>0</v>
@@ -2865,24 +2922,27 @@
         <v>0</v>
       </c>
       <c r="O9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>39</v>
+      <c r="E10" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>0</v>
@@ -2902,8 +2962,8 @@
       <c r="K10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>23</v>
+      <c r="L10" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="M10" s="1" t="n">
         <v>0</v>
@@ -2912,18 +2972,21 @@
         <v>0</v>
       </c>
       <c r="O10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>0</v>
@@ -2947,8 +3010,8 @@
       <c r="K11" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>23</v>
+      <c r="L11" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="M11" s="1" t="n">
         <v>0</v>
@@ -2957,18 +3020,21 @@
         <v>0</v>
       </c>
       <c r="O11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>0</v>
@@ -2992,8 +3058,8 @@
       <c r="K12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>23</v>
+      <c r="L12" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="M12" s="1" t="n">
         <v>0</v>
@@ -3002,18 +3068,21 @@
         <v>0</v>
       </c>
       <c r="O12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>0</v>
@@ -3037,8 +3106,8 @@
       <c r="K13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>23</v>
+      <c r="L13" s="7" t="s">
+        <v>54</v>
       </c>
       <c r="M13" s="1" t="n">
         <v>0</v>
@@ -3047,24 +3116,27 @@
         <v>0</v>
       </c>
       <c r="O13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>47</v>
+      <c r="E14" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="F14" s="1" t="n">
         <v>0</v>
@@ -3084,8 +3156,8 @@
       <c r="K14" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L14" s="1" t="s">
-        <v>23</v>
+      <c r="L14" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="M14" s="1" t="n">
         <v>0</v>
@@ -3094,24 +3166,27 @@
         <v>0</v>
       </c>
       <c r="O14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>47</v>
+      <c r="E15" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="F15" s="1" t="n">
         <v>0</v>
@@ -3131,8 +3206,8 @@
       <c r="K15" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>23</v>
+      <c r="L15" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="M15" s="1" t="n">
         <v>0</v>
@@ -3143,38 +3218,45 @@
       <c r="O15" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="P15" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="6"/>
+      <c r="L16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B17" s="0"/>
       <c r="C17" s="0"/>
       <c r="D17" s="0"/>
-      <c r="E17" s="0"/>
+      <c r="E17" s="8"/>
       <c r="F17" s="0"/>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
       <c r="I17" s="0"/>
       <c r="J17" s="0"/>
       <c r="K17" s="0"/>
-      <c r="L17" s="0"/>
+      <c r="L17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>54</v>
+      <c r="E18" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="F18" s="1" t="n">
         <v>0</v>
@@ -3194,8 +3276,8 @@
       <c r="K18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L18" s="6" t="s">
-        <v>55</v>
+      <c r="L18" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="M18" s="1" t="n">
         <v>0</v>
@@ -3206,25 +3288,28 @@
       <c r="O18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P18" s="4" t="s">
-        <v>56</v>
+      <c r="P18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>54</v>
+      <c r="E19" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="F19" s="1" t="n">
         <v>0</v>
@@ -3244,8 +3329,8 @@
       <c r="K19" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L19" s="6" t="s">
-        <v>55</v>
+      <c r="L19" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="M19" s="1" t="n">
         <v>0</v>
@@ -3254,24 +3339,27 @@
         <v>0</v>
       </c>
       <c r="O19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>28</v>
+      <c r="E20" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="F20" s="1" t="n">
         <v>0</v>
@@ -3291,8 +3379,8 @@
       <c r="K20" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L20" s="6" t="s">
-        <v>55</v>
+      <c r="L20" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="M20" s="1" t="n">
         <v>0</v>
@@ -3301,18 +3389,21 @@
         <v>0</v>
       </c>
       <c r="O20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>1</v>
@@ -3336,8 +3427,8 @@
       <c r="K21" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L21" s="6" t="s">
-        <v>55</v>
+      <c r="L21" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="M21" s="1" t="n">
         <v>0</v>
@@ -3346,24 +3437,27 @@
         <v>0</v>
       </c>
       <c r="O21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P21" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>64</v>
+      <c r="E22" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="F22" s="1" t="n">
         <v>1</v>
@@ -3383,8 +3477,8 @@
       <c r="K22" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L22" s="1" t="s">
-        <v>65</v>
+      <c r="L22" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="M22" s="1" t="n">
         <v>0</v>
@@ -3393,24 +3487,27 @@
         <v>0</v>
       </c>
       <c r="O22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P22" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>64</v>
+      <c r="E23" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="F23" s="1" t="n">
         <v>0</v>
@@ -3430,8 +3527,8 @@
       <c r="K23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L23" s="1" t="s">
-        <v>65</v>
+      <c r="L23" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="M23" s="1" t="n">
         <v>0</v>
@@ -3440,18 +3537,21 @@
         <v>0</v>
       </c>
       <c r="O23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P23" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>1</v>
@@ -3475,8 +3575,8 @@
       <c r="K24" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L24" s="6" t="s">
-        <v>55</v>
+      <c r="L24" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="M24" s="1" t="n">
         <v>0</v>
@@ -3485,24 +3585,27 @@
         <v>0</v>
       </c>
       <c r="O24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P24" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D25" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>39</v>
+      <c r="E25" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F25" s="1" t="n">
         <v>0</v>
@@ -3522,8 +3625,8 @@
       <c r="K25" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L25" s="6" t="s">
-        <v>55</v>
+      <c r="L25" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="M25" s="1" t="n">
         <v>0</v>
@@ -3532,24 +3635,27 @@
         <v>0</v>
       </c>
       <c r="O25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D26" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>36</v>
+      <c r="E26" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="F26" s="1" t="n">
         <v>0</v>
@@ -3569,8 +3675,8 @@
       <c r="K26" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L26" s="6" t="s">
-        <v>55</v>
+      <c r="L26" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="M26" s="1" t="n">
         <v>0</v>
@@ -3581,27 +3687,36 @@
       <c r="O26" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="P26" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E27" s="6"/>
+      <c r="L27" s="7"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E28" s="6"/>
+      <c r="L28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>47</v>
+        <v>88</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="F29" s="1" t="n">
         <v>0</v>
@@ -3621,8 +3736,8 @@
       <c r="K29" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L29" s="1" t="s">
-        <v>78</v>
+      <c r="L29" s="7" t="s">
+        <v>89</v>
       </c>
       <c r="M29" s="1" t="n">
         <v>0</v>
@@ -3631,24 +3746,27 @@
         <v>0</v>
       </c>
       <c r="O29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>47</v>
+        <v>88</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="F30" s="1" t="n">
         <v>0</v>
@@ -3668,8 +3786,8 @@
       <c r="K30" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L30" s="1" t="s">
-        <v>78</v>
+      <c r="L30" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="M30" s="1" t="n">
         <v>0</v>
@@ -3680,24 +3798,33 @@
       <c r="O30" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="P30" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E31" s="6"/>
+      <c r="L31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="E32" s="6"/>
+      <c r="L32" s="7"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="1" t="n">
@@ -3712,14 +3839,14 @@
       <c r="I33" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="J33" s="1" t="n">
+      <c r="J33" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K33" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L33" s="6" t="s">
-        <v>82</v>
+      <c r="L33" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="M33" s="1" t="n">
         <v>1</v>
@@ -3728,21 +3855,24 @@
         <v>0</v>
       </c>
       <c r="O33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P33" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="1" t="n">
@@ -3757,14 +3887,14 @@
       <c r="I34" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J34" s="1" t="n">
+      <c r="J34" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K34" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L34" s="6" t="s">
-        <v>82</v>
+      <c r="L34" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="M34" s="1" t="n">
         <v>0</v>
@@ -3774,20 +3904,23 @@
       </c>
       <c r="O34" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="P34" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="1" t="n">
@@ -3802,14 +3935,14 @@
       <c r="I35" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="J35" s="6" t="n">
+      <c r="J35" s="7" t="n">
         <v>1</v>
       </c>
       <c r="K35" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L35" s="1" t="s">
-        <v>23</v>
+      <c r="L35" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="M35" s="1" t="n">
         <v>0</v>
@@ -3818,75 +3951,103 @@
         <v>1</v>
       </c>
       <c r="O35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P35" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E36" s="6"/>
-      <c r="J36" s="6"/>
+      <c r="J36" s="7"/>
+      <c r="L36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
+      <c r="A37" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="J37" s="7"/>
+      <c r="L37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="L38" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="M38" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="N38" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="O38" s="1" t="s">
-        <v>77</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="6"/>
+      <c r="F38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L38" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="M38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P38" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="L39" s="7"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J40" s="7"/>
+      <c r="L40" s="7"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L41" s="7"/>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L42" s="7"/>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L43" s="7"/>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L44" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:U1"/>
+    <mergeCell ref="D1:V1"/>
     <mergeCell ref="A37:E37"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
figuring out ALU sigs
</commit_message>
<xml_diff>
--- a/SingleCycleProcessor_ControlSignals.xlsx
+++ b/SingleCycleProcessor_ControlSignals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="105">
   <si>
     <t xml:space="preserve">Instruction</t>
   </si>
@@ -94,12 +94,12 @@
     <t xml:space="preserve">"100001"</t>
   </si>
   <si>
-    <t xml:space="preserve">0010 [A + B]</t>
-  </si>
-  <si>
     <t xml:space="preserve">0001 [add]</t>
   </si>
   <si>
+    <t xml:space="preserve">0001 [R-type]</t>
+  </si>
+  <si>
     <t xml:space="preserve">add</t>
   </si>
   <si>
@@ -112,9 +112,6 @@
     <t xml:space="preserve">"100100"</t>
   </si>
   <si>
-    <t xml:space="preserve">0000 []</t>
-  </si>
-  <si>
     <t xml:space="preserve">0010 [and]</t>
   </si>
   <si>
@@ -145,9 +142,6 @@
     <t xml:space="preserve">"100101"</t>
   </si>
   <si>
-    <t xml:space="preserve">0001 []</t>
-  </si>
-  <si>
     <t xml:space="preserve">0101 [or]</t>
   </si>
   <si>
@@ -157,9 +151,6 @@
     <t xml:space="preserve">"101010"</t>
   </si>
   <si>
-    <t xml:space="preserve">0111 []</t>
-  </si>
-  <si>
     <t xml:space="preserve">0110 [slt]</t>
   </si>
   <si>
@@ -193,9 +184,6 @@
     <t xml:space="preserve">"100010"</t>
   </si>
   <si>
-    <t xml:space="preserve">0110 []</t>
-  </si>
-  <si>
     <t xml:space="preserve">1010 [sub]</t>
   </si>
   <si>
@@ -217,27 +205,7 @@
     <t xml:space="preserve">"------"</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">0010 </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[A + B]</t>
-    </r>
+    <t xml:space="preserve">0010 [addi]</t>
   </si>
   <si>
     <t xml:space="preserve">Note: other signals you may have must be correctly assigned for the add; if you redefined these signals, you probably will need to change the sample values</t>
@@ -255,6 +223,9 @@
     <t xml:space="preserve">"001100"</t>
   </si>
   <si>
+    <t xml:space="preserve">0011 [andi]</t>
+  </si>
+  <si>
     <t xml:space="preserve">lui</t>
   </si>
   <si>
@@ -264,12 +235,12 @@
     <t xml:space="preserve">1101 [lui]</t>
   </si>
   <si>
+    <t xml:space="preserve">0100 [lui]</t>
+  </si>
+  <si>
     <t xml:space="preserve">lw</t>
   </si>
   <si>
-    <t xml:space="preserve">0010 []</t>
-  </si>
-  <si>
     <t xml:space="preserve">0000 [LS]</t>
   </si>
   <si>
@@ -288,18 +259,27 @@
     <t xml:space="preserve">“------”</t>
   </si>
   <si>
+    <t xml:space="preserve">0101 [xori]</t>
+  </si>
+  <si>
     <t xml:space="preserve">slti</t>
   </si>
   <si>
     <t xml:space="preserve">"001010"</t>
   </si>
   <si>
+    <t xml:space="preserve">0110 [slti]</t>
+  </si>
+  <si>
     <t xml:space="preserve">ori</t>
   </si>
   <si>
     <t xml:space="preserve">"001101"</t>
   </si>
   <si>
+    <t xml:space="preserve">0111 [ori]</t>
+  </si>
+  <si>
     <t xml:space="preserve">beq</t>
   </si>
   <si>
@@ -312,6 +292,9 @@
     <t xml:space="preserve">1011 [beq]</t>
   </si>
   <si>
+    <t xml:space="preserve">1000 [beq]</t>
+  </si>
+  <si>
     <t xml:space="preserve">bne</t>
   </si>
   <si>
@@ -321,15 +304,24 @@
     <t xml:space="preserve">1100 [bne]</t>
   </si>
   <si>
+    <t xml:space="preserve">1001 [bne]</t>
+  </si>
+  <si>
     <t xml:space="preserve">j</t>
   </si>
   <si>
     <t xml:space="preserve">1110 [Jumps]</t>
   </si>
   <si>
+    <t xml:space="preserve">1010 [j]</t>
+  </si>
+  <si>
     <t xml:space="preserve">jal</t>
   </si>
   <si>
+    <t xml:space="preserve">1011 [jal]</t>
+  </si>
+  <si>
     <t xml:space="preserve">jr</t>
   </si>
   <si>
@@ -337,6 +329,9 @@
   </si>
   <si>
     <t xml:space="preserve">“010100”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1111[halt??]</t>
   </si>
   <si>
     <t xml:space="preserve">1111 [halt]??</t>
@@ -429,7 +424,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -454,16 +449,8 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -471,6 +458,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -498,7 +489,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K11" activeCellId="0" sqref="K11"/>
+      <selection pane="bottomRight" activeCell="L42" activeCellId="0" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -513,7 +504,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.88"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.5"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="13" style="1" width="10.8"/>
   </cols>
   <sheetData>
@@ -656,7 +647,7 @@
       <c r="K4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="6" t="s">
         <v>25</v>
       </c>
       <c r="M4" s="1" t="n">
@@ -1710,7 +1701,7 @@
       <c r="K5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="6" t="s">
         <v>25</v>
       </c>
       <c r="M5" s="1" t="n">
@@ -2764,8 +2755,8 @@
       <c r="K6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L6" s="7" t="s">
-        <v>31</v>
+      <c r="L6" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="M6" s="1" t="n">
         <v>0</v>
@@ -2782,20 +2773,20 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="6" t="n">
-        <v>1100</v>
-      </c>
       <c r="F7" s="1" t="n">
         <v>0</v>
       </c>
@@ -2814,8 +2805,8 @@
       <c r="K7" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L7" s="7" t="s">
-        <v>34</v>
+      <c r="L7" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="M7" s="1" t="n">
         <v>0</v>
@@ -2832,18 +2823,20 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="6"/>
       <c r="F8" s="1" t="n">
         <v>0</v>
       </c>
@@ -2862,8 +2855,8 @@
       <c r="K8" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L8" s="7" t="s">
-        <v>38</v>
+      <c r="L8" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="M8" s="1" t="n">
         <v>0</v>
@@ -2880,20 +2873,20 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="F9" s="1" t="n">
         <v>0</v>
       </c>
@@ -2912,8 +2905,8 @@
       <c r="K9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L9" s="7" t="s">
-        <v>42</v>
+      <c r="L9" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="M9" s="1" t="n">
         <v>0</v>
@@ -2930,19 +2923,19 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>0</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>0</v>
@@ -2962,8 +2955,8 @@
       <c r="K10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L10" s="7" t="s">
-        <v>46</v>
+      <c r="L10" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="M10" s="1" t="n">
         <v>0</v>
@@ -2980,7 +2973,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>22</v>
@@ -2991,7 +2984,9 @@
       <c r="D11" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E11" s="6"/>
+      <c r="E11" s="6" t="s">
+        <v>45</v>
+      </c>
       <c r="F11" s="1" t="n">
         <v>0</v>
       </c>
@@ -3010,8 +3005,8 @@
       <c r="K11" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L11" s="7" t="s">
-        <v>48</v>
+      <c r="L11" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="M11" s="1" t="n">
         <v>0</v>
@@ -3028,18 +3023,20 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E12" s="6"/>
+      <c r="E12" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="F12" s="1" t="n">
         <v>0</v>
       </c>
@@ -3058,8 +3055,8 @@
       <c r="K12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L12" s="7" t="s">
-        <v>51</v>
+      <c r="L12" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="M12" s="1" t="n">
         <v>0</v>
@@ -3076,18 +3073,20 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E13" s="6"/>
+      <c r="E13" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="F13" s="1" t="n">
         <v>0</v>
       </c>
@@ -3106,8 +3105,8 @@
       <c r="K13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L13" s="7" t="s">
-        <v>54</v>
+      <c r="L13" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="M13" s="1" t="n">
         <v>0</v>
@@ -3124,19 +3123,19 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>0</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F14" s="1" t="n">
         <v>0</v>
@@ -3156,8 +3155,8 @@
       <c r="K14" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L14" s="7" t="s">
-        <v>58</v>
+      <c r="L14" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="M14" s="1" t="n">
         <v>0</v>
@@ -3174,19 +3173,19 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>0</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F15" s="1" t="n">
         <v>0</v>
@@ -3206,8 +3205,8 @@
       <c r="K15" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L15" s="7" t="s">
-        <v>58</v>
+      <c r="L15" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="M15" s="1" t="n">
         <v>0</v>
@@ -3224,92 +3223,92 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E16" s="6"/>
-      <c r="L16" s="7"/>
+      <c r="L16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B17" s="0"/>
       <c r="C17" s="0"/>
       <c r="D17" s="0"/>
-      <c r="E17" s="8"/>
+      <c r="E17" s="7"/>
       <c r="F17" s="0"/>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
       <c r="I17" s="0"/>
       <c r="J17" s="0"/>
       <c r="K17" s="0"/>
-      <c r="L17" s="9"/>
+      <c r="L17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L18" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="4" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="F19" s="1" t="n">
         <v>0</v>
@@ -3329,8 +3328,8 @@
       <c r="K19" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L19" s="7" t="s">
-        <v>25</v>
+      <c r="L19" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="M19" s="1" t="n">
         <v>0</v>
@@ -3347,13 +3346,13 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>1</v>
@@ -3379,8 +3378,8 @@
       <c r="K20" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L20" s="7" t="s">
-        <v>31</v>
+      <c r="L20" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="M20" s="1" t="n">
         <v>0</v>
@@ -3397,38 +3396,40 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G21" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H21" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J21" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L21" s="10" t="s">
-        <v>73</v>
       </c>
       <c r="M21" s="1" t="n">
         <v>0</v>
@@ -3445,19 +3446,19 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="D22" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F22" s="1" t="n">
         <v>1</v>
@@ -3477,8 +3478,8 @@
       <c r="K22" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L22" s="7" t="s">
-        <v>76</v>
+      <c r="L22" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="M22" s="1" t="n">
         <v>0</v>
@@ -3495,19 +3496,19 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F23" s="1" t="n">
         <v>0</v>
@@ -3527,8 +3528,8 @@
       <c r="K23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L23" s="7" t="s">
-        <v>76</v>
+      <c r="L23" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="M23" s="1" t="n">
         <v>0</v>
@@ -3545,38 +3546,40 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" s="8" t="s">
         <v>79</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G24" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H24" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I24" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J24" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K24" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L24" s="7" t="s">
-        <v>38</v>
       </c>
       <c r="M24" s="1" t="n">
         <v>0</v>
@@ -3593,40 +3596,40 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I25" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L25" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="M25" s="1" t="n">
         <v>0</v>
@@ -3643,40 +3646,40 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F26" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G26" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I26" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J26" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K26" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L26" s="7" t="s">
-        <v>42</v>
       </c>
       <c r="M26" s="1" t="n">
         <v>0</v>
@@ -3693,14 +3696,14 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E27" s="6"/>
-      <c r="L27" s="7"/>
+      <c r="L27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E28" s="6"/>
-      <c r="L28" s="7"/>
+      <c r="L28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
@@ -3710,13 +3713,13 @@
         <v>87</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>88</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>57</v>
+        <v>89</v>
       </c>
       <c r="F29" s="1" t="n">
         <v>0</v>
@@ -3736,8 +3739,8 @@
       <c r="K29" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L29" s="7" t="s">
-        <v>89</v>
+      <c r="L29" s="6" t="s">
+        <v>90</v>
       </c>
       <c r="M29" s="1" t="n">
         <v>0</v>
@@ -3754,19 +3757,19 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>88</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
       <c r="F30" s="1" t="n">
         <v>0</v>
@@ -3786,8 +3789,8 @@
       <c r="K30" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L30" s="7" t="s">
-        <v>92</v>
+      <c r="L30" s="6" t="s">
+        <v>94</v>
       </c>
       <c r="M30" s="1" t="n">
         <v>0</v>
@@ -3804,29 +3807,31 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E31" s="6"/>
-      <c r="L31" s="7"/>
+      <c r="L31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E32" s="6"/>
-      <c r="L32" s="7"/>
+      <c r="L32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E33" s="6"/>
+      <c r="E33" s="6" t="s">
+        <v>96</v>
+      </c>
       <c r="F33" s="1" t="n">
         <v>0</v>
       </c>
@@ -3839,14 +3844,14 @@
       <c r="I33" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="J33" s="7" t="n">
+      <c r="J33" s="6" t="n">
         <v>0</v>
       </c>
       <c r="K33" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L33" s="7" t="s">
-        <v>94</v>
+      <c r="L33" s="6" t="s">
+        <v>97</v>
       </c>
       <c r="M33" s="1" t="n">
         <v>1</v>
@@ -3863,18 +3868,20 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E34" s="6"/>
+      <c r="E34" s="6" t="s">
+        <v>96</v>
+      </c>
       <c r="F34" s="1" t="n">
         <v>0</v>
       </c>
@@ -3887,14 +3894,14 @@
       <c r="I34" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J34" s="7" t="n">
+      <c r="J34" s="6" t="n">
         <v>0</v>
       </c>
       <c r="K34" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L34" s="7" t="s">
-        <v>94</v>
+      <c r="L34" s="6" t="s">
+        <v>99</v>
       </c>
       <c r="M34" s="1" t="n">
         <v>0</v>
@@ -3911,18 +3918,20 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E35" s="6"/>
+      <c r="E35" s="6" t="s">
+        <v>96</v>
+      </c>
       <c r="F35" s="1" t="n">
         <v>0</v>
       </c>
@@ -3935,14 +3944,14 @@
       <c r="I35" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="J35" s="7" t="n">
+      <c r="J35" s="6" t="n">
         <v>1</v>
       </c>
       <c r="K35" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L35" s="7" t="s">
-        <v>94</v>
+      <c r="L35" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="M35" s="1" t="n">
         <v>0</v>
@@ -3959,34 +3968,38 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E36" s="6"/>
-      <c r="J36" s="7"/>
-      <c r="L36" s="7"/>
+      <c r="J36" s="6"/>
+      <c r="L36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="J37" s="7"/>
-      <c r="L37" s="7"/>
+      <c r="E37" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J37" s="6"/>
+      <c r="L37" s="6"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D38" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E38" s="6"/>
+      <c r="E38" s="9" t="s">
+        <v>103</v>
+      </c>
       <c r="F38" s="1" t="n">
         <v>0</v>
       </c>
@@ -3999,14 +4012,14 @@
       <c r="I38" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="J38" s="7" t="n">
+      <c r="J38" s="6" t="n">
         <v>0</v>
       </c>
       <c r="K38" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L38" s="6" t="s">
-        <v>99</v>
+      <c r="L38" s="9" t="s">
+        <v>104</v>
       </c>
       <c r="M38" s="1" t="n">
         <v>0</v>
@@ -4022,25 +4035,25 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="L39" s="7"/>
+      <c r="E39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="L39" s="6"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J40" s="7"/>
-      <c r="L40" s="7"/>
+      <c r="J40" s="6"/>
+      <c r="L40" s="6"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L41" s="7"/>
+      <c r="L41" s="6"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L42" s="7"/>
+      <c r="L42" s="6"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L43" s="7"/>
+      <c r="L43" s="6"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L44" s="7"/>
+      <c r="L44" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
i hate this design
</commit_message>
<xml_diff>
--- a/SingleCycleProcessor_ControlSignals.xlsx
+++ b/SingleCycleProcessor_ControlSignals.xlsx
@@ -424,7 +424,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -453,15 +453,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -489,7 +493,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L42" activeCellId="0" sqref="L42"/>
+      <selection pane="bottomRight" activeCell="I32" activeCellId="0" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -647,7 +651,7 @@
       <c r="K4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="7" t="s">
         <v>25</v>
       </c>
       <c r="M4" s="1" t="n">
@@ -1701,7 +1705,7 @@
       <c r="K5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="L5" s="7" t="s">
         <v>25</v>
       </c>
       <c r="M5" s="1" t="n">
@@ -2755,7 +2759,7 @@
       <c r="K6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="L6" s="7" t="s">
         <v>25</v>
       </c>
       <c r="M6" s="1" t="n">
@@ -2805,7 +2809,7 @@
       <c r="K7" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="L7" s="7" t="s">
         <v>25</v>
       </c>
       <c r="M7" s="1" t="n">
@@ -2855,7 +2859,7 @@
       <c r="K8" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="L8" s="7" t="s">
         <v>25</v>
       </c>
       <c r="M8" s="1" t="n">
@@ -2905,7 +2909,7 @@
       <c r="K9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L9" s="6" t="s">
+      <c r="L9" s="7" t="s">
         <v>25</v>
       </c>
       <c r="M9" s="1" t="n">
@@ -2955,7 +2959,7 @@
       <c r="K10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L10" s="6" t="s">
+      <c r="L10" s="7" t="s">
         <v>25</v>
       </c>
       <c r="M10" s="1" t="n">
@@ -3005,7 +3009,7 @@
       <c r="K11" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L11" s="6" t="s">
+      <c r="L11" s="7" t="s">
         <v>25</v>
       </c>
       <c r="M11" s="1" t="n">
@@ -3055,7 +3059,7 @@
       <c r="K12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L12" s="6" t="s">
+      <c r="L12" s="7" t="s">
         <v>25</v>
       </c>
       <c r="M12" s="1" t="n">
@@ -3105,7 +3109,7 @@
       <c r="K13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L13" s="6" t="s">
+      <c r="L13" s="7" t="s">
         <v>25</v>
       </c>
       <c r="M13" s="1" t="n">
@@ -3155,7 +3159,7 @@
       <c r="K14" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L14" s="6" t="s">
+      <c r="L14" s="7" t="s">
         <v>25</v>
       </c>
       <c r="M14" s="1" t="n">
@@ -3205,7 +3209,7 @@
       <c r="K15" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L15" s="6" t="s">
+      <c r="L15" s="7" t="s">
         <v>25</v>
       </c>
       <c r="M15" s="1" t="n">
@@ -3223,7 +3227,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E16" s="6"/>
-      <c r="L16" s="6"/>
+      <c r="L16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
@@ -3232,14 +3236,14 @@
       <c r="B17" s="0"/>
       <c r="C17" s="0"/>
       <c r="D17" s="0"/>
-      <c r="E17" s="7"/>
+      <c r="E17" s="8"/>
       <c r="F17" s="0"/>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
       <c r="I17" s="0"/>
       <c r="J17" s="0"/>
       <c r="K17" s="0"/>
-      <c r="L17" s="7"/>
+      <c r="L17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
@@ -3275,7 +3279,7 @@
       <c r="K18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L18" s="6" t="s">
+      <c r="L18" s="7" t="s">
         <v>61</v>
       </c>
       <c r="M18" s="1" t="n">
@@ -3328,7 +3332,7 @@
       <c r="K19" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L19" s="6" t="s">
+      <c r="L19" s="7" t="s">
         <v>61</v>
       </c>
       <c r="M19" s="1" t="n">
@@ -3378,7 +3382,7 @@
       <c r="K20" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L20" s="6" t="s">
+      <c r="L20" s="7" t="s">
         <v>67</v>
       </c>
       <c r="M20" s="1" t="n">
@@ -3407,7 +3411,7 @@
       <c r="D21" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="10" t="s">
         <v>70</v>
       </c>
       <c r="F21" s="1" t="n">
@@ -3428,7 +3432,7 @@
       <c r="K21" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L21" s="6" t="s">
+      <c r="L21" s="7" t="s">
         <v>71</v>
       </c>
       <c r="M21" s="1" t="n">
@@ -3478,7 +3482,7 @@
       <c r="K22" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L22" s="6" t="s">
+      <c r="L22" s="7" t="s">
         <v>73</v>
       </c>
       <c r="M22" s="1" t="n">
@@ -3528,7 +3532,7 @@
       <c r="K23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L23" s="6" t="s">
+      <c r="L23" s="7" t="s">
         <v>73</v>
       </c>
       <c r="M23" s="1" t="n">
@@ -3578,7 +3582,7 @@
       <c r="K24" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L24" s="8" t="s">
+      <c r="L24" s="7" t="s">
         <v>79</v>
       </c>
       <c r="M24" s="1" t="n">
@@ -3628,7 +3632,7 @@
       <c r="K25" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L25" s="6" t="s">
+      <c r="L25" s="7" t="s">
         <v>82</v>
       </c>
       <c r="M25" s="1" t="n">
@@ -3678,7 +3682,7 @@
       <c r="K26" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L26" s="6" t="s">
+      <c r="L26" s="7" t="s">
         <v>85</v>
       </c>
       <c r="M26" s="1" t="n">
@@ -3696,14 +3700,14 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E27" s="6"/>
-      <c r="L27" s="6"/>
+      <c r="L27" s="7"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E28" s="6"/>
-      <c r="L28" s="6"/>
+      <c r="L28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
@@ -3739,7 +3743,7 @@
       <c r="K29" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L29" s="6" t="s">
+      <c r="L29" s="7" t="s">
         <v>90</v>
       </c>
       <c r="M29" s="1" t="n">
@@ -3789,7 +3793,7 @@
       <c r="K30" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L30" s="6" t="s">
+      <c r="L30" s="7" t="s">
         <v>94</v>
       </c>
       <c r="M30" s="1" t="n">
@@ -3807,14 +3811,14 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E31" s="6"/>
-      <c r="L31" s="6"/>
+      <c r="L31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E32" s="6"/>
-      <c r="L32" s="6"/>
+      <c r="L32" s="7"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
@@ -3850,7 +3854,7 @@
       <c r="K33" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L33" s="6" t="s">
+      <c r="L33" s="7" t="s">
         <v>97</v>
       </c>
       <c r="M33" s="1" t="n">
@@ -3900,7 +3904,7 @@
       <c r="K34" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L34" s="6" t="s">
+      <c r="L34" s="7" t="s">
         <v>99</v>
       </c>
       <c r="M34" s="1" t="n">
@@ -3950,7 +3954,7 @@
       <c r="K35" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L35" s="6" t="s">
+      <c r="L35" s="7" t="s">
         <v>25</v>
       </c>
       <c r="M35" s="1" t="n">
@@ -3969,7 +3973,7 @@
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E36" s="6"/>
       <c r="J36" s="6"/>
-      <c r="L36" s="6"/>
+      <c r="L36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
@@ -3982,7 +3986,7 @@
         <v>24</v>
       </c>
       <c r="J37" s="6"/>
-      <c r="L37" s="6"/>
+      <c r="L37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
@@ -3997,7 +4001,7 @@
       <c r="D38" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="E38" s="7" t="s">
         <v>103</v>
       </c>
       <c r="F38" s="1" t="n">
@@ -4018,7 +4022,7 @@
       <c r="K38" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L38" s="9" t="s">
+      <c r="L38" s="7" t="s">
         <v>104</v>
       </c>
       <c r="M38" s="1" t="n">

</xml_diff>

<commit_message>
created ALU control tb
</commit_message>
<xml_diff>
--- a/SingleCycleProcessor_ControlSignals.xlsx
+++ b/SingleCycleProcessor_ControlSignals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="100">
   <si>
     <t xml:space="preserve">Instruction</t>
   </si>
@@ -310,18 +310,9 @@
     <t xml:space="preserve">j</t>
   </si>
   <si>
-    <t xml:space="preserve">1110 [Jumps]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1010 [j]</t>
-  </si>
-  <si>
     <t xml:space="preserve">jal</t>
   </si>
   <si>
-    <t xml:space="preserve">1011 [jal]</t>
-  </si>
-  <si>
     <t xml:space="preserve">jr</t>
   </si>
   <si>
@@ -329,12 +320,6 @@
   </si>
   <si>
     <t xml:space="preserve">“010100”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1111[halt??]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1111 [halt]??</t>
   </si>
 </sst>
 </file>
@@ -424,7 +409,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -457,16 +442,8 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -493,7 +470,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I32" activeCellId="0" sqref="I32"/>
+      <selection pane="bottomRight" activeCell="E29" activeCellId="1" sqref="L38 E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3236,14 +3213,14 @@
       <c r="B17" s="0"/>
       <c r="C17" s="0"/>
       <c r="D17" s="0"/>
-      <c r="E17" s="8"/>
+      <c r="E17" s="0"/>
       <c r="F17" s="0"/>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
       <c r="I17" s="0"/>
       <c r="J17" s="0"/>
       <c r="K17" s="0"/>
-      <c r="L17" s="9"/>
+      <c r="L17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
@@ -3411,7 +3388,7 @@
       <c r="D21" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="6" t="s">
         <v>70</v>
       </c>
       <c r="F21" s="1" t="n">
@@ -3833,9 +3810,7 @@
       <c r="D33" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E33" s="6" t="s">
-        <v>96</v>
-      </c>
+      <c r="E33" s="6"/>
       <c r="F33" s="1" t="n">
         <v>0</v>
       </c>
@@ -3854,9 +3829,7 @@
       <c r="K33" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L33" s="7" t="s">
-        <v>97</v>
-      </c>
+      <c r="L33" s="7"/>
       <c r="M33" s="1" t="n">
         <v>1</v>
       </c>
@@ -3872,7 +3845,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>50</v>
@@ -3883,9 +3856,7 @@
       <c r="D34" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E34" s="6" t="s">
-        <v>96</v>
-      </c>
+      <c r="E34" s="6"/>
       <c r="F34" s="1" t="n">
         <v>0</v>
       </c>
@@ -3904,9 +3875,7 @@
       <c r="K34" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L34" s="7" t="s">
-        <v>99</v>
-      </c>
+      <c r="L34" s="7"/>
       <c r="M34" s="1" t="n">
         <v>0</v>
       </c>
@@ -3922,7 +3891,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>22</v>
@@ -3933,9 +3902,7 @@
       <c r="D35" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E35" s="6" t="s">
-        <v>96</v>
-      </c>
+      <c r="E35" s="6"/>
       <c r="F35" s="1" t="n">
         <v>0</v>
       </c>
@@ -3954,9 +3921,7 @@
       <c r="K35" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L35" s="7" t="s">
-        <v>25</v>
-      </c>
+      <c r="L35" s="7"/>
       <c r="M35" s="1" t="n">
         <v>0</v>
       </c>
@@ -3977,7 +3942,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -3993,7 +3958,7 @@
         <v>16</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>60</v>
@@ -4001,9 +3966,7 @@
       <c r="D38" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E38" s="7" t="s">
-        <v>103</v>
-      </c>
+      <c r="E38" s="7"/>
       <c r="F38" s="1" t="n">
         <v>0</v>
       </c>
@@ -4022,9 +3985,7 @@
       <c r="K38" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L38" s="7" t="s">
-        <v>104</v>
-      </c>
+      <c r="L38" s="7"/>
       <c r="M38" s="1" t="n">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
updated signal sheet with which inst are functional
</commit_message>
<xml_diff>
--- a/SingleCycleProcessor_ControlSignals.xlsx
+++ b/SingleCycleProcessor_ControlSignals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="121">
   <si>
     <t xml:space="preserve">Instruction</t>
   </si>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">Halt</t>
   </si>
   <si>
-    <t xml:space="preserve">Note: these are example control signals from the text and your skeleton code; you will need to add more control signals; you may rename any control signals, except those given in the skeleton code.</t>
+    <t xml:space="preserve">Functional</t>
   </si>
   <si>
     <t xml:space="preserve">R-type</t>
@@ -151,6 +151,9 @@
     <t xml:space="preserve">00101[slt]</t>
   </si>
   <si>
+    <t xml:space="preserve">Fails 1 case</t>
+  </si>
+  <si>
     <t xml:space="preserve">sll</t>
   </si>
   <si>
@@ -203,9 +206,6 @@
   </si>
   <si>
     <t xml:space="preserve">01010[addi]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Note: other signals you may have must be correctly assigned for the add; if you redefined these signals, you probably will need to change the sample values</t>
   </si>
   <si>
     <t xml:space="preserve">addiu</t>
@@ -392,7 +392,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -423,19 +423,25 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -478,7 +484,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -507,11 +513,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -572,7 +590,7 @@
       <rgbColor rgb="FFFFD8CE"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF81D41A"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -599,11 +617,11 @@
   <dimension ref="A1:AMJ68"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="D58" activeCellId="0" sqref="D58"/>
+      <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="L23" activeCellId="0" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -615,7 +633,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.88"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.8"/>
@@ -714,18 +732,6 @@
       <c r="J3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="Q3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -775,6 +781,7 @@
       <c r="P4" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q4" s="7"/>
       <c r="U4" s="0"/>
       <c r="V4" s="0"/>
       <c r="W4" s="0"/>
@@ -1827,6 +1834,7 @@
       <c r="P5" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q5" s="7"/>
       <c r="U5" s="0"/>
       <c r="V5" s="0"/>
       <c r="W5" s="0"/>
@@ -2879,6 +2887,7 @@
       <c r="P6" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -2927,6 +2936,7 @@
       <c r="P7" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -2975,6 +2985,7 @@
       <c r="P8" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -3023,6 +3034,7 @@
       <c r="P9" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -3071,10 +3083,13 @@
       <c r="P10" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q10" s="8" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>22</v>
@@ -3105,7 +3120,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M11" s="1" t="n">
         <v>0</v>
@@ -3119,16 +3134,17 @@
       <c r="P11" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>0</v>
@@ -3153,7 +3169,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M12" s="1" t="n">
         <v>0</v>
@@ -3167,16 +3183,17 @@
       <c r="P12" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>0</v>
@@ -3201,7 +3218,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M13" s="1" t="n">
         <v>0</v>
@@ -3215,16 +3232,17 @@
       <c r="P13" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>0</v>
@@ -3249,7 +3267,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M14" s="1" t="n">
         <v>0</v>
@@ -3263,16 +3281,17 @@
       <c r="P14" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>0</v>
@@ -3297,7 +3316,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M15" s="1" t="n">
         <v>0</v>
@@ -3311,6 +3330,7 @@
       <c r="P15" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E16" s="6"/>
@@ -3318,7 +3338,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B17" s="0"/>
       <c r="C17" s="0"/>
@@ -3334,13 +3354,13 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>1</v>
@@ -3365,7 +3385,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="M18" s="1" t="n">
         <v>0</v>
@@ -3379,9 +3399,7 @@
       <c r="P18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q18" s="4" t="s">
-        <v>61</v>
-      </c>
+      <c r="Q18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
@@ -3391,7 +3409,7 @@
         <v>63</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>1</v>
@@ -3416,7 +3434,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="M19" s="1" t="n">
         <v>0</v>
@@ -3430,6 +3448,7 @@
       <c r="P19" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
@@ -3439,7 +3458,7 @@
         <v>65</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>1</v>
@@ -3478,6 +3497,7 @@
       <c r="P20" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
@@ -3487,7 +3507,7 @@
         <v>68</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>1</v>
@@ -3526,16 +3546,17 @@
       <c r="P21" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>1</v>
@@ -3574,6 +3595,7 @@
       <c r="P22" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q22" s="8"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
@@ -3583,7 +3605,7 @@
         <v>73</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>1</v>
@@ -3622,6 +3644,7 @@
       <c r="P23" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q23" s="8"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
@@ -3670,6 +3693,9 @@
       <c r="P24" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q24" s="8" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
@@ -3679,7 +3705,7 @@
         <v>79</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D25" s="1" t="n">
         <v>1</v>
@@ -3718,6 +3744,7 @@
       <c r="P25" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q25" s="8"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
@@ -3727,7 +3754,7 @@
         <v>82</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D26" s="1" t="n">
         <v>1</v>
@@ -3766,6 +3793,7 @@
       <c r="P26" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q26" s="7"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E27" s="6"/>
@@ -3786,7 +3814,7 @@
         <v>85</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>86</v>
@@ -3824,6 +3852,9 @@
       </c>
       <c r="P29" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="Q29" s="8" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3834,7 +3865,7 @@
         <v>89</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>86</v>
@@ -3873,6 +3904,7 @@
       <c r="P30" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q30" s="8"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E31" s="6"/>
@@ -3890,10 +3922,10 @@
         <v>90</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>86</v>
@@ -3932,16 +3964,17 @@
       <c r="P33" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>86</v>
@@ -3980,6 +4013,7 @@
       <c r="P34" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q34" s="8"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
@@ -3989,7 +4023,7 @@
         <v>22</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>86</v>
@@ -4028,6 +4062,7 @@
       <c r="P35" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q35" s="8"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E36" s="6"/>
@@ -4055,7 +4090,7 @@
         <v>96</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D38" s="1" t="n">
         <v>0</v>
@@ -4110,25 +4145,25 @@
       <c r="C41" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="E41" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="F41" s="7" t="s">
+      <c r="F41" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="G41" s="7" t="s">
+      <c r="G41" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="H41" s="7" t="s">
+      <c r="H41" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="I41" s="7" t="s">
+      <c r="I41" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="J41" s="7" t="s">
+      <c r="J41" s="10" t="s">
         <v>103</v>
       </c>
       <c r="L41" s="6"/>
@@ -4144,16 +4179,16 @@
       <c r="D42" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="E42" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="F42" s="8" t="n">
+      <c r="F42" s="11" t="n">
         <v>0</v>
       </c>
       <c r="G42" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="H42" s="8" t="n">
+      <c r="H42" s="11" t="n">
         <v>0</v>
       </c>
       <c r="I42" s="6" t="n">
@@ -4176,16 +4211,16 @@
       <c r="D43" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="E43" s="8" t="s">
+      <c r="E43" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="F43" s="8" t="n">
+      <c r="F43" s="11" t="n">
         <v>0</v>
       </c>
       <c r="G43" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="H43" s="8" t="n">
+      <c r="H43" s="11" t="n">
         <v>0</v>
       </c>
       <c r="I43" s="6" t="n">
@@ -4205,7 +4240,7 @@
       <c r="C44" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D44" s="8" t="n">
+      <c r="D44" s="11" t="n">
         <v>0</v>
       </c>
       <c r="E44" s="6" t="s">
@@ -4217,7 +4252,7 @@
       <c r="G44" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="H44" s="8" t="n">
+      <c r="H44" s="11" t="n">
         <v>0</v>
       </c>
       <c r="I44" s="6" t="n">
@@ -4237,7 +4272,7 @@
       <c r="C45" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D45" s="8" t="n">
+      <c r="D45" s="11" t="n">
         <v>0</v>
       </c>
       <c r="E45" s="6" t="s">
@@ -4249,7 +4284,7 @@
       <c r="G45" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="H45" s="8" t="n">
+      <c r="H45" s="11" t="n">
         <v>0</v>
       </c>
       <c r="I45" s="6" t="n">
@@ -4269,7 +4304,7 @@
       <c r="C46" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="D46" s="8" t="n">
+      <c r="D46" s="11" t="n">
         <v>0</v>
       </c>
       <c r="E46" s="6" t="s">
@@ -4281,7 +4316,7 @@
       <c r="G46" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="H46" s="8" t="n">
+      <c r="H46" s="11" t="n">
         <v>0</v>
       </c>
       <c r="I46" s="6" t="n">
@@ -4301,7 +4336,7 @@
       <c r="C47" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="D47" s="8" t="n">
+      <c r="D47" s="11" t="n">
         <v>0</v>
       </c>
       <c r="E47" s="6" t="s">
@@ -4313,7 +4348,7 @@
       <c r="G47" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="H47" s="8" t="n">
+      <c r="H47" s="11" t="n">
         <v>0</v>
       </c>
       <c r="I47" s="6" t="n">
@@ -4333,7 +4368,7 @@
       <c r="C48" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="D48" s="8" t="n">
+      <c r="D48" s="11" t="n">
         <v>0</v>
       </c>
       <c r="E48" s="6" t="s">
@@ -4345,7 +4380,7 @@
       <c r="G48" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="H48" s="8" t="n">
+      <c r="H48" s="11" t="n">
         <v>0</v>
       </c>
       <c r="I48" s="6" t="n">
@@ -4360,21 +4395,21 @@
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0"/>
       <c r="B49" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="D49" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" s="8" t="s">
+      <c r="D49" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="F49" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G49" s="8" t="n">
+      <c r="F49" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" s="11" t="n">
         <v>0</v>
       </c>
       <c r="H49" s="6" t="n">
@@ -4392,21 +4427,21 @@
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0"/>
       <c r="B50" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="D50" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E50" s="8" t="s">
+      <c r="D50" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="F50" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G50" s="8" t="n">
+      <c r="F50" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" s="11" t="n">
         <v>0</v>
       </c>
       <c r="H50" s="6" t="n">
@@ -4424,21 +4459,21 @@
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0"/>
       <c r="B51" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="D51" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E51" s="8" t="s">
+      <c r="D51" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="F51" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G51" s="8" t="n">
+      <c r="F51" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" s="11" t="n">
         <v>0</v>
       </c>
       <c r="H51" s="6" t="n">
@@ -4456,7 +4491,7 @@
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0"/>
       <c r="B52" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>118</v>
@@ -4464,16 +4499,16 @@
       <c r="D52" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="E52" s="8" t="s">
+      <c r="E52" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="F52" s="8" t="n">
+      <c r="F52" s="11" t="n">
         <v>0</v>
       </c>
       <c r="G52" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="H52" s="8" t="n">
+      <c r="H52" s="11" t="n">
         <v>0</v>
       </c>
       <c r="I52" s="6" t="n">
@@ -4488,7 +4523,7 @@
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0"/>
       <c r="B53" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>119</v>
@@ -4496,16 +4531,16 @@
       <c r="D53" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="E53" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="F53" s="8" t="n">
+      <c r="F53" s="11" t="n">
         <v>0</v>
       </c>
       <c r="G53" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="H53" s="8" t="n">
+      <c r="H53" s="11" t="n">
         <v>0</v>
       </c>
       <c r="I53" s="6" t="n">
@@ -4525,16 +4560,16 @@
       <c r="C54" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="D54" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E54" s="8" t="s">
+      <c r="D54" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="F54" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G54" s="8" t="n">
+      <c r="F54" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" s="11" t="n">
         <v>0</v>
       </c>
       <c r="H54" s="6" t="n">
@@ -4728,7 +4763,7 @@
       <c r="L67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D68" s="9"/>
+      <c r="D68" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
fixed slt and slti
</commit_message>
<xml_diff>
--- a/SingleCycleProcessor_ControlSignals.xlsx
+++ b/SingleCycleProcessor_ControlSignals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="123">
   <si>
     <t xml:space="preserve">Instruction</t>
   </si>
@@ -151,111 +151,111 @@
     <t xml:space="preserve">00101[slt]</t>
   </si>
   <si>
+    <t xml:space="preserve">sll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00110[sll]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">srl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"000010"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00111[srl]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"000011"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01000[sra]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"100010"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01001[sub]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"100011"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I-Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"001000"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"------"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01010[addi]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addiu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"001001"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">andi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"001100"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01011[andi]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lui</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"001111"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01100[lui]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01101[lw]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"101011"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xori</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“001110”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“------”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01110[xori]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fails 1 case</t>
   </si>
   <si>
-    <t xml:space="preserve">sll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00110[sll]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">srl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"000010"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00111[srl]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"000011"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01000[sra]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"100010"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01001[sub]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">subu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"100011"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I-Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">addi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"001000"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"------"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01010[addi]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">addiu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"001001"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">andi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"001100"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01011[andi]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lui</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"001111"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01100[lui]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01101[lw]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"101011"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xori</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“001110”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“------”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01110[xori]</t>
-  </si>
-  <si>
     <t xml:space="preserve">slti</t>
   </si>
   <si>
@@ -365,6 +365,12 @@
   </si>
   <si>
     <t xml:space="preserve">“0110”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1(was 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should signed be 1?</t>
   </si>
   <si>
     <t xml:space="preserve">“0111”</t>
@@ -484,7 +490,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -517,6 +523,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -530,6 +540,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -617,11 +631,11 @@
   <dimension ref="A1:AMJ68"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D30" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="L23" activeCellId="0" sqref="L23"/>
+      <selection pane="bottomLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+      <selection pane="bottomRight" activeCell="K57" activeCellId="0" sqref="K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3083,13 +3097,11 @@
       <c r="P10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q10" s="8" t="s">
-        <v>43</v>
-      </c>
+      <c r="Q10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>22</v>
@@ -3120,7 +3132,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M11" s="1" t="n">
         <v>0</v>
@@ -3138,13 +3150,13 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>0</v>
@@ -3169,7 +3181,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M12" s="1" t="n">
         <v>0</v>
@@ -3187,13 +3199,13 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>0</v>
@@ -3218,7 +3230,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M13" s="1" t="n">
         <v>0</v>
@@ -3232,17 +3244,17 @@
       <c r="P13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q13" s="8"/>
+      <c r="Q13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>0</v>
@@ -3267,7 +3279,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M14" s="1" t="n">
         <v>0</v>
@@ -3285,13 +3297,13 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>0</v>
@@ -3316,7 +3328,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M15" s="1" t="n">
         <v>0</v>
@@ -3338,7 +3350,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" s="0"/>
       <c r="C17" s="0"/>
@@ -3354,13 +3366,13 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>1</v>
@@ -3385,7 +3397,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M18" s="1" t="n">
         <v>0</v>
@@ -3399,17 +3411,17 @@
       <c r="P18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q18" s="9"/>
+      <c r="Q18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="C19" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>1</v>
@@ -3434,7 +3446,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M19" s="1" t="n">
         <v>0</v>
@@ -3452,13 +3464,13 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="C20" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>1</v>
@@ -3483,7 +3495,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M20" s="1" t="n">
         <v>0</v>
@@ -3501,13 +3513,13 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="C21" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>1</v>
@@ -3532,7 +3544,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M21" s="1" t="n">
         <v>0</v>
@@ -3550,13 +3562,13 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>1</v>
@@ -3581,7 +3593,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M22" s="1" t="n">
         <v>0</v>
@@ -3595,17 +3607,17 @@
       <c r="P22" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q22" s="8"/>
+      <c r="Q22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="C23" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>1</v>
@@ -3630,7 +3642,7 @@
         <v>0</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M23" s="1" t="n">
         <v>0</v>
@@ -3644,17 +3656,17 @@
       <c r="P23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q23" s="8"/>
+      <c r="Q23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>1</v>
@@ -3679,22 +3691,22 @@
         <v>0</v>
       </c>
       <c r="L24" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="M24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="9" t="s">
         <v>77</v>
-      </c>
-      <c r="M24" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N24" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O24" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P24" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="8" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3705,7 +3717,7 @@
         <v>79</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D25" s="1" t="n">
         <v>1</v>
@@ -3744,7 +3756,7 @@
       <c r="P25" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q25" s="8"/>
+      <c r="Q25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
@@ -3754,7 +3766,7 @@
         <v>82</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D26" s="1" t="n">
         <v>1</v>
@@ -3814,7 +3826,7 @@
         <v>85</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>86</v>
@@ -3853,8 +3865,8 @@
       <c r="P29" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q29" s="8" t="s">
-        <v>43</v>
+      <c r="Q29" s="9" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3865,7 +3877,7 @@
         <v>89</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>86</v>
@@ -3904,7 +3916,7 @@
       <c r="P30" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q30" s="8"/>
+      <c r="Q30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E31" s="6"/>
@@ -3922,10 +3934,10 @@
         <v>90</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>86</v>
@@ -3964,17 +3976,17 @@
       <c r="P33" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q33" s="8"/>
+      <c r="Q33" s="9"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>86</v>
@@ -4013,7 +4025,7 @@
       <c r="P34" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q34" s="8"/>
+      <c r="Q34" s="9"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
@@ -4023,7 +4035,7 @@
         <v>22</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>86</v>
@@ -4062,7 +4074,7 @@
       <c r="P35" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q35" s="8"/>
+      <c r="Q35" s="9"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E36" s="6"/>
@@ -4090,7 +4102,7 @@
         <v>96</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D38" s="1" t="n">
         <v>0</v>
@@ -4145,25 +4157,25 @@
       <c r="C41" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D41" s="10" t="s">
+      <c r="D41" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="E41" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="F41" s="10" t="s">
+      <c r="F41" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="G41" s="10" t="s">
+      <c r="G41" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="H41" s="10" t="s">
+      <c r="H41" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="I41" s="10" t="s">
+      <c r="I41" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="J41" s="10" t="s">
+      <c r="J41" s="11" t="s">
         <v>103</v>
       </c>
       <c r="L41" s="6"/>
@@ -4179,16 +4191,16 @@
       <c r="D42" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="E42" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="F42" s="11" t="n">
+      <c r="F42" s="12" t="n">
         <v>0</v>
       </c>
       <c r="G42" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="H42" s="11" t="n">
+      <c r="H42" s="12" t="n">
         <v>0</v>
       </c>
       <c r="I42" s="6" t="n">
@@ -4211,16 +4223,16 @@
       <c r="D43" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="E43" s="11" t="s">
+      <c r="E43" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="F43" s="11" t="n">
+      <c r="F43" s="12" t="n">
         <v>0</v>
       </c>
       <c r="G43" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="H43" s="11" t="n">
+      <c r="H43" s="12" t="n">
         <v>0</v>
       </c>
       <c r="I43" s="6" t="n">
@@ -4240,7 +4252,7 @@
       <c r="C44" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D44" s="11" t="n">
+      <c r="D44" s="12" t="n">
         <v>0</v>
       </c>
       <c r="E44" s="6" t="s">
@@ -4252,7 +4264,7 @@
       <c r="G44" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="H44" s="11" t="n">
+      <c r="H44" s="12" t="n">
         <v>0</v>
       </c>
       <c r="I44" s="6" t="n">
@@ -4272,7 +4284,7 @@
       <c r="C45" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D45" s="11" t="n">
+      <c r="D45" s="12" t="n">
         <v>0</v>
       </c>
       <c r="E45" s="6" t="s">
@@ -4284,7 +4296,7 @@
       <c r="G45" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="H45" s="11" t="n">
+      <c r="H45" s="12" t="n">
         <v>0</v>
       </c>
       <c r="I45" s="6" t="n">
@@ -4304,7 +4316,7 @@
       <c r="C46" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="D46" s="11" t="n">
+      <c r="D46" s="12" t="n">
         <v>0</v>
       </c>
       <c r="E46" s="6" t="s">
@@ -4316,7 +4328,7 @@
       <c r="G46" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="H46" s="11" t="n">
+      <c r="H46" s="12" t="n">
         <v>0</v>
       </c>
       <c r="I46" s="6" t="n">
@@ -4336,7 +4348,7 @@
       <c r="C47" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="D47" s="11" t="n">
+      <c r="D47" s="12" t="n">
         <v>0</v>
       </c>
       <c r="E47" s="6" t="s">
@@ -4348,7 +4360,7 @@
       <c r="G47" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="H47" s="11" t="n">
+      <c r="H47" s="12" t="n">
         <v>0</v>
       </c>
       <c r="I47" s="6" t="n">
@@ -4368,8 +4380,8 @@
       <c r="C48" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="D48" s="11" t="n">
-        <v>0</v>
+      <c r="D48" s="13" t="s">
+        <v>115</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>105</v>
@@ -4380,7 +4392,7 @@
       <c r="G48" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="H48" s="11" t="n">
+      <c r="H48" s="12" t="n">
         <v>0</v>
       </c>
       <c r="I48" s="6" t="n">
@@ -4389,27 +4401,29 @@
       <c r="J48" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="K48" s="0"/>
+      <c r="K48" s="0" t="s">
+        <v>116</v>
+      </c>
       <c r="L48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0"/>
       <c r="B49" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D49" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D49" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="F49" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G49" s="11" t="n">
+      <c r="F49" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" s="12" t="n">
         <v>0</v>
       </c>
       <c r="H49" s="6" t="n">
@@ -4427,21 +4441,21 @@
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0"/>
       <c r="B50" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D50" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E50" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D50" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="F50" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G50" s="11" t="n">
+      <c r="F50" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" s="12" t="n">
         <v>0</v>
       </c>
       <c r="H50" s="6" t="n">
@@ -4459,21 +4473,21 @@
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0"/>
       <c r="B51" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="D51" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E51" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="D51" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="F51" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G51" s="11" t="n">
+      <c r="F51" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" s="12" t="n">
         <v>0</v>
       </c>
       <c r="H51" s="6" t="n">
@@ -4491,24 +4505,24 @@
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0"/>
       <c r="B52" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D52" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="E52" s="11" t="s">
+      <c r="E52" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="F52" s="11" t="n">
+      <c r="F52" s="12" t="n">
         <v>0</v>
       </c>
       <c r="G52" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="H52" s="11" t="n">
+      <c r="H52" s="12" t="n">
         <v>0</v>
       </c>
       <c r="I52" s="6" t="n">
@@ -4523,24 +4537,24 @@
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0"/>
       <c r="B53" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D53" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="E53" s="11" t="s">
+      <c r="E53" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="F53" s="11" t="n">
+      <c r="F53" s="12" t="n">
         <v>0</v>
       </c>
       <c r="G53" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="H53" s="11" t="n">
+      <c r="H53" s="12" t="n">
         <v>0</v>
       </c>
       <c r="I53" s="6" t="n">
@@ -4555,21 +4569,21 @@
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0"/>
       <c r="B54" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D54" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E54" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D54" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="F54" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G54" s="11" t="n">
+      <c r="F54" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" s="12" t="n">
         <v>0</v>
       </c>
       <c r="H54" s="6" t="n">
@@ -4763,7 +4777,7 @@
       <c r="L67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D68" s="12"/>
+      <c r="D68" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
fixed xor and xori
</commit_message>
<xml_diff>
--- a/SingleCycleProcessor_ControlSignals.xlsx
+++ b/SingleCycleProcessor_ControlSignals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="122">
   <si>
     <t xml:space="preserve">Instruction</t>
   </si>
@@ -253,39 +253,39 @@
     <t xml:space="preserve">01110[xori]</t>
   </si>
   <si>
+    <t xml:space="preserve">slti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"001010"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01111[stli]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ori</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"001101"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10000[ori]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"000100"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“-”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10001[branch]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fails 1 case</t>
   </si>
   <si>
-    <t xml:space="preserve">slti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"001010"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01111[stli]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ori</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"001101"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10000[ori]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">beq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"000100"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“-”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10001[branch]</t>
-  </si>
-  <si>
     <t xml:space="preserve">bne</t>
   </si>
   <si>
@@ -368,9 +368,6 @@
   </si>
   <si>
     <t xml:space="preserve">1(was 0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Should signed be 1?</t>
   </si>
   <si>
     <t xml:space="preserve">“0111”</t>
@@ -631,11 +628,11 @@
   <dimension ref="A1:AMJ68"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D18" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
-      <selection pane="bottomRight" activeCell="K57" activeCellId="0" sqref="K57"/>
+      <selection pane="bottomLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="bottomRight" activeCell="K48" activeCellId="0" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3705,16 +3702,14 @@
       <c r="P24" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q24" s="9" t="s">
-        <v>77</v>
-      </c>
+      <c r="Q24" s="8"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>59</v>
@@ -3742,7 +3737,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M25" s="1" t="n">
         <v>0</v>
@@ -3756,14 +3751,14 @@
       <c r="P25" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q25" s="9"/>
+      <c r="Q25" s="8"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>59</v>
@@ -3791,7 +3786,7 @@
         <v>0</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M26" s="1" t="n">
         <v>0</v>
@@ -3820,16 +3815,16 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="1" t="n">
@@ -3851,22 +3846,22 @@
         <v>1</v>
       </c>
       <c r="L29" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="M29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="9" t="s">
         <v>87</v>
-      </c>
-      <c r="M29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="9" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3880,7 +3875,7 @@
         <v>59</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="1" t="n">
@@ -3902,7 +3897,7 @@
         <v>1</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M30" s="1" t="n">
         <v>0</v>
@@ -3940,7 +3935,7 @@
         <v>59</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="1" t="n">
@@ -3989,7 +3984,7 @@
         <v>59</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="1" t="n">
@@ -4038,7 +4033,7 @@
         <v>58</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="1" t="n">
@@ -4401,9 +4396,7 @@
       <c r="J48" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="K48" s="0" t="s">
-        <v>116</v>
-      </c>
+      <c r="K48" s="0"/>
       <c r="L48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4412,7 +4405,7 @@
         <v>43</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D49" s="12" t="n">
         <v>0</v>
@@ -4444,7 +4437,7 @@
         <v>45</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D50" s="12" t="n">
         <v>0</v>
@@ -4476,7 +4469,7 @@
         <v>48</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D51" s="12" t="n">
         <v>0</v>
@@ -4508,7 +4501,7 @@
         <v>51</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D52" s="6" t="n">
         <v>1</v>
@@ -4540,7 +4533,7 @@
         <v>54</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D53" s="6" t="n">
         <v>1</v>
@@ -4572,7 +4565,7 @@
         <v>66</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D54" s="12" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
load and store work
</commit_message>
<xml_diff>
--- a/SingleCycleProcessor_ControlSignals.xlsx
+++ b/SingleCycleProcessor_ControlSignals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="122">
   <si>
     <t xml:space="preserve">Instruction</t>
   </si>
@@ -235,6 +235,9 @@
     <t xml:space="preserve">01101[lw]</t>
   </si>
   <si>
+    <t xml:space="preserve">Fails 1 case</t>
+  </si>
+  <si>
     <t xml:space="preserve">sw</t>
   </si>
   <si>
@@ -281,9 +284,6 @@
   </si>
   <si>
     <t xml:space="preserve">10001[branch]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fails 1 case</t>
   </si>
   <si>
     <t xml:space="preserve">bne</t>
@@ -524,12 +524,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -632,7 +632,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
-      <selection pane="bottomRight" activeCell="K48" activeCellId="0" sqref="K48"/>
+      <selection pane="bottomRight" activeCell="R22" activeCellId="0" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3241,7 +3241,7 @@
       <c r="P13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q13" s="9"/>
+      <c r="Q13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
@@ -3408,7 +3408,7 @@
       <c r="P18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q18" s="10"/>
+      <c r="Q18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
@@ -3604,14 +3604,16 @@
       <c r="P22" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q22" s="9"/>
+      <c r="Q22" s="10" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>59</v>
@@ -3653,17 +3655,17 @@
       <c r="P23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q23" s="9"/>
+      <c r="Q23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>1</v>
@@ -3688,7 +3690,7 @@
         <v>0</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M24" s="1" t="n">
         <v>0</v>
@@ -3706,10 +3708,10 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>59</v>
@@ -3737,7 +3739,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M25" s="1" t="n">
         <v>0</v>
@@ -3755,10 +3757,10 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>59</v>
@@ -3786,7 +3788,7 @@
         <v>0</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M26" s="1" t="n">
         <v>0</v>
@@ -3815,16 +3817,16 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="1" t="n">
@@ -3846,7 +3848,7 @@
         <v>1</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M29" s="1" t="n">
         <v>0</v>
@@ -3860,8 +3862,8 @@
       <c r="P29" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q29" s="9" t="s">
-        <v>87</v>
+      <c r="Q29" s="10" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3875,7 +3877,7 @@
         <v>59</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="1" t="n">
@@ -3897,7 +3899,7 @@
         <v>1</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M30" s="1" t="n">
         <v>0</v>
@@ -3911,7 +3913,7 @@
       <c r="P30" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q30" s="9"/>
+      <c r="Q30" s="10"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E31" s="6"/>
@@ -3935,7 +3937,7 @@
         <v>59</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="1" t="n">
@@ -3971,7 +3973,7 @@
       <c r="P33" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q33" s="9"/>
+      <c r="Q33" s="10"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
@@ -3984,7 +3986,7 @@
         <v>59</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="1" t="n">
@@ -4020,7 +4022,7 @@
       <c r="P34" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q34" s="9"/>
+      <c r="Q34" s="10"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
@@ -4033,7 +4035,7 @@
         <v>58</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="1" t="n">
@@ -4069,7 +4071,7 @@
       <c r="P35" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q35" s="9"/>
+      <c r="Q35" s="10"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E36" s="6"/>

</xml_diff>

<commit_message>
fixed load and store and updated sig sheet
</commit_message>
<xml_diff>
--- a/SingleCycleProcessor_ControlSignals.xlsx
+++ b/SingleCycleProcessor_ControlSignals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="122">
   <si>
     <t xml:space="preserve">Instruction</t>
   </si>
@@ -235,55 +235,55 @@
     <t xml:space="preserve">01101[lw]</t>
   </si>
   <si>
+    <t xml:space="preserve">sw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"101011"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xori</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“001110”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“------”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01110[xori]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"001010"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01111[stli]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ori</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"001101"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10000[ori]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"000100"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“-”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10001[branch]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fails 1 case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"101011"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xori</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“001110”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“------”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01110[xori]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">slti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"001010"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01111[stli]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ori</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"001101"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10000[ori]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">beq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"000100"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“-”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10001[branch]</t>
   </si>
   <si>
     <t xml:space="preserve">bne</t>
@@ -628,11 +628,11 @@
   <dimension ref="A1:AMJ68"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
-      <selection pane="bottomRight" activeCell="R22" activeCellId="0" sqref="R22"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="Q22" activeCellId="0" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3604,16 +3604,14 @@
       <c r="P22" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q22" s="10" t="s">
-        <v>71</v>
-      </c>
+      <c r="Q22" s="8"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>59</v>
@@ -3655,17 +3653,17 @@
       <c r="P23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q23" s="10"/>
+      <c r="Q23" s="8"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>1</v>
@@ -3690,7 +3688,7 @@
         <v>0</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M24" s="1" t="n">
         <v>0</v>
@@ -3708,10 +3706,10 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>59</v>
@@ -3739,7 +3737,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M25" s="1" t="n">
         <v>0</v>
@@ -3757,10 +3755,10 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>59</v>
@@ -3788,7 +3786,7 @@
         <v>0</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M26" s="1" t="n">
         <v>0</v>
@@ -3817,16 +3815,16 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="1" t="n">
@@ -3848,22 +3846,22 @@
         <v>1</v>
       </c>
       <c r="L29" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="M29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="10" t="s">
         <v>87</v>
-      </c>
-      <c r="M29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="10" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3877,7 +3875,7 @@
         <v>59</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="1" t="n">
@@ -3899,7 +3897,7 @@
         <v>1</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M30" s="1" t="n">
         <v>0</v>
@@ -3937,7 +3935,7 @@
         <v>59</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="1" t="n">
@@ -3986,7 +3984,7 @@
         <v>59</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="1" t="n">
@@ -4035,7 +4033,7 @@
         <v>58</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="1" t="n">

</xml_diff>

<commit_message>
fixed jump address and jump instr
</commit_message>
<xml_diff>
--- a/SingleCycleProcessor_ControlSignals.xlsx
+++ b/SingleCycleProcessor_ControlSignals.xlsx
@@ -427,7 +427,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -448,8 +448,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFD7D7"/>
+        <bgColor rgb="FFFFD8CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFD8CE"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFD7D7"/>
       </patternFill>
     </fill>
   </fills>
@@ -487,7 +493,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -532,15 +538,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -577,7 +587,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFFFD7D7"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -628,11 +638,11 @@
   <dimension ref="A1:AMJ68"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q22" activeCellId="0" sqref="Q22"/>
+      <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="L44" activeCellId="0" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3971,7 +3981,7 @@
       <c r="P33" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q33" s="10"/>
+      <c r="Q33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
@@ -4099,41 +4109,41 @@
       <c r="C38" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E38" s="6"/>
-      <c r="F38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J38" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L38" s="6" t="s">
+      <c r="D38" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="12"/>
+      <c r="F38" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L38" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="M38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P38" s="1" t="n">
+      <c r="M38" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O38" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P38" s="11" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4152,25 +4162,25 @@
       <c r="C41" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D41" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="E41" s="11" t="s">
+      <c r="E41" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="F41" s="11" t="s">
+      <c r="F41" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="G41" s="11" t="s">
+      <c r="G41" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="H41" s="11" t="s">
+      <c r="H41" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="I41" s="11" t="s">
+      <c r="I41" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="J41" s="11" t="s">
+      <c r="J41" s="13" t="s">
         <v>103</v>
       </c>
       <c r="L41" s="6"/>
@@ -4186,16 +4196,16 @@
       <c r="D42" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E42" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="F42" s="12" t="n">
+      <c r="F42" s="14" t="n">
         <v>0</v>
       </c>
       <c r="G42" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="H42" s="12" t="n">
+      <c r="H42" s="14" t="n">
         <v>0</v>
       </c>
       <c r="I42" s="6" t="n">
@@ -4218,16 +4228,16 @@
       <c r="D43" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="E43" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="F43" s="12" t="n">
+      <c r="F43" s="14" t="n">
         <v>0</v>
       </c>
       <c r="G43" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="H43" s="12" t="n">
+      <c r="H43" s="14" t="n">
         <v>0</v>
       </c>
       <c r="I43" s="6" t="n">
@@ -4247,7 +4257,7 @@
       <c r="C44" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D44" s="12" t="n">
+      <c r="D44" s="14" t="n">
         <v>0</v>
       </c>
       <c r="E44" s="6" t="s">
@@ -4259,7 +4269,7 @@
       <c r="G44" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="H44" s="12" t="n">
+      <c r="H44" s="14" t="n">
         <v>0</v>
       </c>
       <c r="I44" s="6" t="n">
@@ -4279,7 +4289,7 @@
       <c r="C45" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D45" s="12" t="n">
+      <c r="D45" s="14" t="n">
         <v>0</v>
       </c>
       <c r="E45" s="6" t="s">
@@ -4291,7 +4301,7 @@
       <c r="G45" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="H45" s="12" t="n">
+      <c r="H45" s="14" t="n">
         <v>0</v>
       </c>
       <c r="I45" s="6" t="n">
@@ -4311,7 +4321,7 @@
       <c r="C46" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="D46" s="12" t="n">
+      <c r="D46" s="14" t="n">
         <v>0</v>
       </c>
       <c r="E46" s="6" t="s">
@@ -4323,7 +4333,7 @@
       <c r="G46" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="H46" s="12" t="n">
+      <c r="H46" s="14" t="n">
         <v>0</v>
       </c>
       <c r="I46" s="6" t="n">
@@ -4343,7 +4353,7 @@
       <c r="C47" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="D47" s="12" t="n">
+      <c r="D47" s="14" t="n">
         <v>0</v>
       </c>
       <c r="E47" s="6" t="s">
@@ -4355,7 +4365,7 @@
       <c r="G47" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="H47" s="12" t="n">
+      <c r="H47" s="14" t="n">
         <v>0</v>
       </c>
       <c r="I47" s="6" t="n">
@@ -4375,7 +4385,7 @@
       <c r="C48" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="D48" s="6" t="s">
         <v>115</v>
       </c>
       <c r="E48" s="6" t="s">
@@ -4387,7 +4397,7 @@
       <c r="G48" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="H48" s="12" t="n">
+      <c r="H48" s="14" t="n">
         <v>0</v>
       </c>
       <c r="I48" s="6" t="n">
@@ -4407,16 +4417,16 @@
       <c r="C49" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="D49" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" s="12" t="s">
+      <c r="D49" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="F49" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="G49" s="12" t="n">
+      <c r="F49" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" s="14" t="n">
         <v>0</v>
       </c>
       <c r="H49" s="6" t="n">
@@ -4439,16 +4449,16 @@
       <c r="C50" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="D50" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E50" s="12" t="s">
+      <c r="D50" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="F50" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="G50" s="12" t="n">
+      <c r="F50" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" s="14" t="n">
         <v>0</v>
       </c>
       <c r="H50" s="6" t="n">
@@ -4471,16 +4481,16 @@
       <c r="C51" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="D51" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E51" s="12" t="s">
+      <c r="D51" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="F51" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="G51" s="12" t="n">
+      <c r="F51" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" s="14" t="n">
         <v>0</v>
       </c>
       <c r="H51" s="6" t="n">
@@ -4506,16 +4516,16 @@
       <c r="D52" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="E52" s="12" t="s">
+      <c r="E52" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="F52" s="12" t="n">
+      <c r="F52" s="14" t="n">
         <v>0</v>
       </c>
       <c r="G52" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="H52" s="12" t="n">
+      <c r="H52" s="14" t="n">
         <v>0</v>
       </c>
       <c r="I52" s="6" t="n">
@@ -4538,16 +4548,16 @@
       <c r="D53" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="E53" s="12" t="s">
+      <c r="E53" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="F53" s="12" t="n">
+      <c r="F53" s="14" t="n">
         <v>0</v>
       </c>
       <c r="G53" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="H53" s="12" t="n">
+      <c r="H53" s="14" t="n">
         <v>0</v>
       </c>
       <c r="I53" s="6" t="n">
@@ -4567,16 +4577,16 @@
       <c r="C54" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="D54" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E54" s="12" t="s">
+      <c r="D54" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="F54" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="G54" s="12" t="n">
+      <c r="F54" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" s="14" t="n">
         <v>0</v>
       </c>
       <c r="H54" s="6" t="n">
@@ -4770,7 +4780,7 @@
       <c r="L67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D68" s="14"/>
+      <c r="D68" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
its working babygit add .!
</commit_message>
<xml_diff>
--- a/SingleCycleProcessor_ControlSignals.xlsx
+++ b/SingleCycleProcessor_ControlSignals.xlsx
@@ -298,7 +298,7 @@
     <t xml:space="preserve">jal</t>
   </si>
   <si>
-    <t xml:space="preserve">Jal_5.s</t>
+    <t xml:space="preserve">Fails 1 case</t>
   </si>
   <si>
     <t xml:space="preserve">jr</t>
@@ -638,11 +638,11 @@
   <dimension ref="A1:AMJ68"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S37" activeCellId="0" sqref="S37"/>
+      <selection pane="bottomRight" activeCell="Q30" activeCellId="0" sqref="Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3919,7 +3919,7 @@
       <c r="P30" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q30" s="7"/>
+      <c r="Q30" s="8"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E31" s="6"/>
@@ -4028,8 +4028,7 @@
       <c r="P34" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q34" s="10"/>
-      <c r="R34" s="1" t="s">
+      <c r="Q34" s="10" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated tbs and report
</commit_message>
<xml_diff>
--- a/SingleCycleProcessor_ControlSignals.xlsx
+++ b/SingleCycleProcessor_ControlSignals.xlsx
@@ -73,6 +73,9 @@
     <t xml:space="preserve">Halt</t>
   </si>
   <si>
+    <t xml:space="preserve">ZeroSign</t>
+  </si>
+  <si>
     <t xml:space="preserve">Functional</t>
   </si>
   <si>
@@ -296,9 +299,6 @@
   </si>
   <si>
     <t xml:space="preserve">jal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fails 1 case</t>
   </si>
   <si>
     <t xml:space="preserve">jr</t>
@@ -427,7 +427,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -438,12 +438,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF81D41A"/>
         <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
     <fill>
@@ -493,7 +487,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -534,15 +528,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -550,7 +540,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -637,12 +627,12 @@
   </sheetPr>
   <dimension ref="A1:AMJ68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q30" activeCellId="0" sqref="Q30"/>
+      <selection pane="bottomRight" activeCell="T29" activeCellId="0" sqref="T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -693,6 +683,7 @@
       <c r="T1" s="3"/>
       <c r="U1" s="3"/>
       <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
@@ -737,33 +728,36 @@
       <c r="P2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="E3" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q3" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="R3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>0</v>
@@ -788,7 +782,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M4" s="1" t="n">
         <v>0</v>
@@ -802,8 +796,10 @@
       <c r="P4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q4" s="7"/>
-      <c r="U4" s="0"/>
+      <c r="Q4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R4" s="7"/>
       <c r="V4" s="0"/>
       <c r="W4" s="0"/>
       <c r="X4" s="0"/>
@@ -1810,13 +1806,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>0</v>
@@ -1841,7 +1837,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M5" s="1" t="n">
         <v>0</v>
@@ -1855,8 +1851,10 @@
       <c r="P5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q5" s="7"/>
-      <c r="U5" s="0"/>
+      <c r="Q5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" s="7"/>
       <c r="V5" s="0"/>
       <c r="W5" s="0"/>
       <c r="X5" s="0"/>
@@ -2863,13 +2861,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>0</v>
@@ -2894,7 +2892,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M6" s="1" t="n">
         <v>0</v>
@@ -2908,17 +2906,20 @@
       <c r="P6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q6" s="7"/>
+      <c r="Q6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>0</v>
@@ -2943,7 +2944,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M7" s="1" t="n">
         <v>0</v>
@@ -2957,17 +2958,20 @@
       <c r="P7" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q7" s="7"/>
+      <c r="Q7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>0</v>
@@ -2992,7 +2996,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M8" s="1" t="n">
         <v>0</v>
@@ -3006,17 +3010,20 @@
       <c r="P8" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q8" s="7"/>
+      <c r="Q8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>0</v>
@@ -3041,7 +3048,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M9" s="1" t="n">
         <v>0</v>
@@ -3055,17 +3062,20 @@
       <c r="P9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q9" s="7"/>
+      <c r="Q9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>0</v>
@@ -3090,7 +3100,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M10" s="1" t="n">
         <v>0</v>
@@ -3104,17 +3114,20 @@
       <c r="P10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q10" s="8"/>
+      <c r="Q10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>0</v>
@@ -3139,7 +3152,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M11" s="1" t="n">
         <v>0</v>
@@ -3153,17 +3166,20 @@
       <c r="P11" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q11" s="7"/>
+      <c r="Q11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>0</v>
@@ -3188,7 +3204,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M12" s="1" t="n">
         <v>0</v>
@@ -3202,17 +3218,20 @@
       <c r="P12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q12" s="7"/>
+      <c r="Q12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>0</v>
@@ -3237,7 +3256,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M13" s="1" t="n">
         <v>0</v>
@@ -3251,17 +3270,20 @@
       <c r="P13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q13" s="8"/>
+      <c r="Q13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>0</v>
@@ -3286,7 +3308,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M14" s="1" t="n">
         <v>0</v>
@@ -3300,17 +3322,20 @@
       <c r="P14" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q14" s="7"/>
+      <c r="Q14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>0</v>
@@ -3335,7 +3360,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M15" s="1" t="n">
         <v>0</v>
@@ -3349,7 +3374,10 @@
       <c r="P15" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q15" s="7"/>
+      <c r="Q15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E16" s="6"/>
@@ -3357,7 +3385,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B17" s="0"/>
       <c r="C17" s="0"/>
@@ -3373,13 +3401,13 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>1</v>
@@ -3404,7 +3432,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="M18" s="1" t="n">
         <v>0</v>
@@ -3418,17 +3446,20 @@
       <c r="P18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q18" s="9"/>
+      <c r="Q18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>1</v>
@@ -3453,7 +3484,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="M19" s="1" t="n">
         <v>0</v>
@@ -3467,17 +3498,20 @@
       <c r="P19" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q19" s="7"/>
+      <c r="Q19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>1</v>
@@ -3502,7 +3536,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M20" s="1" t="n">
         <v>0</v>
@@ -3516,17 +3550,20 @@
       <c r="P20" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q20" s="7"/>
+      <c r="Q20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>1</v>
@@ -3551,7 +3588,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M21" s="1" t="n">
         <v>0</v>
@@ -3565,17 +3602,20 @@
       <c r="P21" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q21" s="7"/>
+      <c r="Q21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>1</v>
@@ -3600,7 +3640,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M22" s="1" t="n">
         <v>0</v>
@@ -3614,17 +3654,20 @@
       <c r="P22" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q22" s="8"/>
+      <c r="Q22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R22" s="8"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>1</v>
@@ -3649,7 +3692,7 @@
         <v>0</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M23" s="1" t="n">
         <v>0</v>
@@ -3663,17 +3706,20 @@
       <c r="P23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q23" s="8"/>
+      <c r="Q23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R23" s="8"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>1</v>
@@ -3698,7 +3744,7 @@
         <v>0</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M24" s="1" t="n">
         <v>0</v>
@@ -3712,17 +3758,20 @@
       <c r="P24" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q24" s="8"/>
+      <c r="Q24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R24" s="8"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D25" s="1" t="n">
         <v>1</v>
@@ -3747,7 +3796,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M25" s="1" t="n">
         <v>0</v>
@@ -3761,17 +3810,20 @@
       <c r="P25" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q25" s="8"/>
+      <c r="Q25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R25" s="8"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D26" s="1" t="n">
         <v>1</v>
@@ -3796,7 +3848,7 @@
         <v>0</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M26" s="1" t="n">
         <v>0</v>
@@ -3810,7 +3862,10 @@
       <c r="P26" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q26" s="7"/>
+      <c r="Q26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R26" s="7"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E27" s="6"/>
@@ -3825,16 +3880,16 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="1" t="n">
@@ -3856,7 +3911,7 @@
         <v>1</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M29" s="1" t="n">
         <v>0</v>
@@ -3870,20 +3925,23 @@
       <c r="P29" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q29" s="8"/>
+      <c r="Q29" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R29" s="8"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="1" t="n">
@@ -3905,7 +3963,7 @@
         <v>1</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M30" s="1" t="n">
         <v>0</v>
@@ -3919,7 +3977,10 @@
       <c r="P30" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q30" s="8"/>
+      <c r="Q30" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R30" s="8"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E31" s="6"/>
@@ -3934,16 +3995,16 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="1" t="n">
@@ -3965,7 +4026,7 @@
         <v>0</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M33" s="1" t="n">
         <v>1</v>
@@ -3979,20 +4040,23 @@
       <c r="P33" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q33" s="8"/>
+      <c r="Q33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="1" t="n">
@@ -4014,7 +4078,7 @@
         <v>0</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M34" s="1" t="n">
         <v>0</v>
@@ -4028,22 +4092,23 @@
       <c r="P34" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q34" s="10" t="s">
-        <v>92</v>
-      </c>
+      <c r="Q34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R34" s="8"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="1" t="n">
@@ -4065,7 +4130,7 @@
         <v>0</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M35" s="1" t="n">
         <v>0</v>
@@ -4079,7 +4144,10 @@
       <c r="P35" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q35" s="8"/>
+      <c r="Q35" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R35" s="8"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E36" s="6"/>
@@ -4107,45 +4175,47 @@
         <v>96</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D38" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E38" s="12"/>
-      <c r="F38" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G38" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H38" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I38" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J38" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="K38" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="L38" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="M38" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="N38" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="O38" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="P38" s="11" t="n">
-        <v>1</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D38" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="11"/>
+      <c r="F38" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L38" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="M38" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O38" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P38" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="7"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E39" s="6"/>
@@ -4162,25 +4232,25 @@
       <c r="C41" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="D41" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="E41" s="13" t="s">
+      <c r="E41" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="F41" s="13" t="s">
+      <c r="F41" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="G41" s="13" t="s">
+      <c r="G41" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="H41" s="13" t="s">
+      <c r="H41" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="I41" s="13" t="s">
+      <c r="I41" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="J41" s="13" t="s">
+      <c r="J41" s="12" t="s">
         <v>103</v>
       </c>
       <c r="L41" s="6"/>
@@ -4188,7 +4258,7 @@
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0"/>
       <c r="B42" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>104</v>
@@ -4196,16 +4266,16 @@
       <c r="D42" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="E42" s="14" t="s">
+      <c r="E42" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="F42" s="14" t="n">
+      <c r="F42" s="13" t="n">
         <v>0</v>
       </c>
       <c r="G42" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="H42" s="14" t="n">
+      <c r="H42" s="13" t="n">
         <v>0</v>
       </c>
       <c r="I42" s="6" t="n">
@@ -4220,7 +4290,7 @@
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0"/>
       <c r="B43" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>106</v>
@@ -4228,16 +4298,16 @@
       <c r="D43" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="E43" s="14" t="s">
+      <c r="E43" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="F43" s="14" t="n">
+      <c r="F43" s="13" t="n">
         <v>0</v>
       </c>
       <c r="G43" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="H43" s="14" t="n">
+      <c r="H43" s="13" t="n">
         <v>0</v>
       </c>
       <c r="I43" s="6" t="n">
@@ -4252,12 +4322,12 @@
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0"/>
       <c r="B44" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D44" s="14" t="n">
+      <c r="D44" s="13" t="n">
         <v>0</v>
       </c>
       <c r="E44" s="6" t="s">
@@ -4269,7 +4339,7 @@
       <c r="G44" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="H44" s="14" t="n">
+      <c r="H44" s="13" t="n">
         <v>0</v>
       </c>
       <c r="I44" s="6" t="n">
@@ -4284,12 +4354,12 @@
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0"/>
       <c r="B45" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D45" s="14" t="n">
+      <c r="D45" s="13" t="n">
         <v>0</v>
       </c>
       <c r="E45" s="6" t="s">
@@ -4301,7 +4371,7 @@
       <c r="G45" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="H45" s="14" t="n">
+      <c r="H45" s="13" t="n">
         <v>0</v>
       </c>
       <c r="I45" s="6" t="n">
@@ -4316,12 +4386,12 @@
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0"/>
       <c r="B46" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="D46" s="14" t="n">
+      <c r="D46" s="13" t="n">
         <v>0</v>
       </c>
       <c r="E46" s="6" t="s">
@@ -4333,7 +4403,7 @@
       <c r="G46" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="H46" s="14" t="n">
+      <c r="H46" s="13" t="n">
         <v>0</v>
       </c>
       <c r="I46" s="6" t="n">
@@ -4348,12 +4418,12 @@
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0"/>
       <c r="B47" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="D47" s="14" t="n">
+      <c r="D47" s="13" t="n">
         <v>0</v>
       </c>
       <c r="E47" s="6" t="s">
@@ -4365,7 +4435,7 @@
       <c r="G47" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="H47" s="14" t="n">
+      <c r="H47" s="13" t="n">
         <v>0</v>
       </c>
       <c r="I47" s="6" t="n">
@@ -4380,7 +4450,7 @@
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0"/>
       <c r="B48" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>114</v>
@@ -4397,7 +4467,7 @@
       <c r="G48" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="H48" s="14" t="n">
+      <c r="H48" s="13" t="n">
         <v>0</v>
       </c>
       <c r="I48" s="6" t="n">
@@ -4412,21 +4482,21 @@
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0"/>
       <c r="B49" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="D49" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" s="14" t="s">
+      <c r="D49" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="F49" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="G49" s="14" t="n">
+      <c r="F49" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" s="13" t="n">
         <v>0</v>
       </c>
       <c r="H49" s="6" t="n">
@@ -4444,21 +4514,21 @@
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0"/>
       <c r="B50" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="D50" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="E50" s="14" t="s">
+      <c r="D50" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="F50" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="G50" s="14" t="n">
+      <c r="F50" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" s="13" t="n">
         <v>0</v>
       </c>
       <c r="H50" s="6" t="n">
@@ -4476,21 +4546,21 @@
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0"/>
       <c r="B51" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="D51" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="E51" s="14" t="s">
+      <c r="D51" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="F51" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="G51" s="14" t="n">
+      <c r="F51" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" s="13" t="n">
         <v>0</v>
       </c>
       <c r="H51" s="6" t="n">
@@ -4508,7 +4578,7 @@
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0"/>
       <c r="B52" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>119</v>
@@ -4516,16 +4586,16 @@
       <c r="D52" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="E52" s="14" t="s">
+      <c r="E52" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="F52" s="14" t="n">
+      <c r="F52" s="13" t="n">
         <v>0</v>
       </c>
       <c r="G52" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="H52" s="14" t="n">
+      <c r="H52" s="13" t="n">
         <v>0</v>
       </c>
       <c r="I52" s="6" t="n">
@@ -4540,7 +4610,7 @@
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0"/>
       <c r="B53" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>120</v>
@@ -4548,16 +4618,16 @@
       <c r="D53" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="E53" s="14" t="s">
+      <c r="E53" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="F53" s="14" t="n">
+      <c r="F53" s="13" t="n">
         <v>0</v>
       </c>
       <c r="G53" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="H53" s="14" t="n">
+      <c r="H53" s="13" t="n">
         <v>0</v>
       </c>
       <c r="I53" s="6" t="n">
@@ -4572,21 +4642,21 @@
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0"/>
       <c r="B54" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="D54" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="E54" s="14" t="s">
+      <c r="D54" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="F54" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="G54" s="14" t="n">
+      <c r="F54" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" s="13" t="n">
         <v>0</v>
       </c>
       <c r="H54" s="6" t="n">
@@ -4780,14 +4850,14 @@
       <c r="L67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D68" s="15"/>
+      <c r="D68" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:V1"/>
+    <mergeCell ref="D1:W1"/>
     <mergeCell ref="A37:E37"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>